<commit_message>
Added support for schema-informed encodings, using the Office Open XML (Strict) schemas. Required linking to xml.xsd to support the http://www.w3.org/XML/1998/namespace, and xml.xsd is now included alongside the Open XML files. Converted all sample files to the newer Office 365 "Strict Open XML" format.
</commit_message>
<xml_diff>
--- a/samples/research.xlsx
+++ b/samples/research.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15" conformance="strict">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr dateCompatibility="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\exify-office\samples\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-12300" yWindow="105" windowWidth="36300" windowHeight="11130"/>
+    <workbookView xWindow="-12300" yWindow="105" windowWidth="36300" windowHeight="11130" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Navy " sheetId="4" r:id="rId1"/>
@@ -17,11 +22,16 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Navy '!$D$1:$K$317</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2714" uniqueCount="1412">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="2714" uniqueCount="1412">
   <si>
     <t>Background: USS MIAMI (SSN 755) suffered fire damage which included environmentally assisted cracking (EAC) to its Ship Service 3000 PSI hydraulic system piping.  Initial scientific investigations of the damaged piping interior has identified burned hard scale and tacky petroleum residue contamination.  This condition is not restorable with existing NAVSEA approved methods.
 Objective: Research, identify and discuss technically achievable novel solutions for the restoration of in-service submarine Ship Service hydraulic system piping by Fleet Maintenance Activity maintenance personnel during a Depot level industrial availability. (1) Investigate methods of inspecting shafts for cracks and surface irregularities without removing the shaft. (2) Investigate the hydraulic  piping off the USS MIAMI that was subjected to Environmentally Assisted Corrosion (EAC)and/or heat and evaluate how these adverse conditions could affect the piping for continued in-service use, should another submarine be subjected to similar conditions in the future.</t>
@@ -5129,8 +5139,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="16">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5265,19 +5275,19 @@
   </fills>
   <borders count="2">
     <border>
-      <left/>
-      <right/>
+      <start/>
+      <end/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <start style="thin">
         <color indexed="64"/>
-      </left>
-      <right style="thin">
+      </start>
+      <end style="thin">
         <color indexed="64"/>
-      </right>
+      </end>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -5433,24 +5443,24 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -5459,7 +5469,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -5483,7 +5493,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -5507,7 +5517,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -5531,7 +5541,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -5555,7 +5565,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -5579,7 +5589,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -5602,7 +5612,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -5612,15 +5622,20 @@
       <color rgb="FF0000FF"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:C299" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowCellStyle="Normal 2" dataCellStyle="Normal 2">
-  <autoFilter ref="A1:C299">
-    <filterColumn colId="1"/>
-    <filterColumn colId="2"/>
-  </autoFilter>
+<table xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" id="6" name="Table6" displayName="Table6" ref="A1:C299" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowCellStyle="Normal 2" dataCellStyle="Normal 2">
+  <autoFilter ref="A1:C299"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Entry Date" dataDxfId="6" dataCellStyle="Normal 2"/>
     <tableColumn id="4" name="NPS Topic Number" dataDxfId="5" dataCellStyle="Normal 2"/>
@@ -5631,10 +5646,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:B14" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2" headerRowCellStyle="Normal 2" dataCellStyle="Normal 2">
-  <autoFilter ref="A1:B14">
-    <filterColumn colId="1"/>
-  </autoFilter>
+<table xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" id="7" name="Table7" displayName="Table7" ref="A1:B14" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2" headerRowCellStyle="Normal 2" dataCellStyle="Normal 2">
+  <autoFilter ref="A1:B14"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Entry Date" dataDxfId="1" dataCellStyle="Normal 2"/>
     <tableColumn id="2" name="NPS Topic Number" dataDxfId="0" dataCellStyle="Normal 2"/>
@@ -5644,7 +5657,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -5686,7 +5699,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5718,9 +5731,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5752,6 +5766,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -5761,22 +5776,22 @@
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <a:gs pos="0%">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
+                <a:tint val="50%"/>
+                <a:satMod val="300%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="35000">
+            <a:gs pos="35%">
               <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:tint val="37%"/>
+                <a:satMod val="300%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100000">
+            <a:gs pos="100%">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="15%"/>
+                <a:satMod val="350%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -5784,22 +5799,22 @@
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <a:gs pos="0%">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
+                <a:shade val="51%"/>
+                <a:satMod val="130%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
+            <a:gs pos="80%">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
+                <a:shade val="93%"/>
+                <a:satMod val="130%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100000">
+            <a:gs pos="100%">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:shade val="94%"/>
+                <a:satMod val="135%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -5810,8 +5825,8 @@
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
+              <a:shade val="95%"/>
+              <a:satMod val="105%"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
@@ -5834,7 +5849,7 @@
           <a:effectLst>
             <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="38%"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -5843,7 +5858,7 @@
           <a:effectLst>
             <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
+                <a:alpha val="35%"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -5852,7 +5867,7 @@
           <a:effectLst>
             <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
+                <a:alpha val="35%"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -5875,47 +5890,47 @@
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <a:gs pos="0%">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="40%"/>
+                <a:satMod val="350%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="40000">
+            <a:gs pos="40%">
               <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="45%"/>
+                <a:shade val="99%"/>
+                <a:satMod val="350%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100000">
+            <a:gs pos="100%">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="20%"/>
+                <a:satMod val="255%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect l="50%" t="-80%" r="50%" b="180%"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <a:gs pos="0%">
               <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
+                <a:tint val="80%"/>
+                <a:satMod val="300%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100000">
+            <a:gs pos="100%">
               <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
+                <a:shade val="30%"/>
+                <a:satMod val="200%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect l="50%" t="50%" r="50%" b="50%"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -5927,15 +5942,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CH318"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A302" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C324" sqref="C324"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" style="3" customWidth="1"/>
     <col min="2" max="3" width="22.42578125" style="3" customWidth="1"/>
@@ -5951,7 +5966,7 @@
     <col min="87" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:86" s="4" customFormat="1" ht="31.5">
+    <row r="1" spans="1:86" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>496</v>
       </c>
@@ -6061,9 +6076,9 @@
       <c r="CG1" s="5"/>
       <c r="CH1" s="5"/>
     </row>
-    <row r="2" spans="1:86" ht="63">
-      <c r="A2" s="22">
-        <v>41757</v>
+    <row r="2" spans="1:86" ht="63" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B2" s="26" t="s">
         <v>561</v>
@@ -6090,9 +6105,9 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="3" spans="1:86" ht="31.5">
-      <c r="A3" s="22">
-        <v>41757</v>
+    <row r="3" spans="1:86" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B3" s="24" t="s">
         <v>562</v>
@@ -6119,9 +6134,9 @@
         <v>432</v>
       </c>
     </row>
-    <row r="4" spans="1:86" ht="47.25">
-      <c r="A4" s="22">
-        <v>41757</v>
+    <row r="4" spans="1:86" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B4" s="24" t="s">
         <v>563</v>
@@ -6148,9 +6163,9 @@
         <v>430</v>
       </c>
     </row>
-    <row r="5" spans="1:86" ht="31.5">
-      <c r="A5" s="22">
-        <v>41757</v>
+    <row r="5" spans="1:86" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B5" s="24" t="s">
         <v>564</v>
@@ -6177,9 +6192,9 @@
         <v>425</v>
       </c>
     </row>
-    <row r="6" spans="1:86" ht="31.5">
-      <c r="A6" s="22">
-        <v>41757</v>
+    <row r="6" spans="1:86" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B6" s="24" t="s">
         <v>565</v>
@@ -6206,9 +6221,9 @@
         <v>423</v>
       </c>
     </row>
-    <row r="7" spans="1:86" ht="31.5">
-      <c r="A7" s="22">
-        <v>41757</v>
+    <row r="7" spans="1:86" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B7" s="24" t="s">
         <v>566</v>
@@ -6235,9 +6250,9 @@
         <v>421</v>
       </c>
     </row>
-    <row r="8" spans="1:86" ht="31.5">
-      <c r="A8" s="22">
-        <v>41757</v>
+    <row r="8" spans="1:86" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B8" s="24" t="s">
         <v>567</v>
@@ -6264,9 +6279,9 @@
         <v>419</v>
       </c>
     </row>
-    <row r="9" spans="1:86" ht="31.5">
-      <c r="A9" s="22">
-        <v>41757</v>
+    <row r="9" spans="1:86" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B9" s="24" t="s">
         <v>568</v>
@@ -6293,9 +6308,9 @@
         <v>417</v>
       </c>
     </row>
-    <row r="10" spans="1:86" ht="31.5">
-      <c r="A10" s="22">
-        <v>41757</v>
+    <row r="10" spans="1:86" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B10" s="24" t="s">
         <v>569</v>
@@ -6322,9 +6337,9 @@
         <v>415</v>
       </c>
     </row>
-    <row r="11" spans="1:86" ht="63">
-      <c r="A11" s="22">
-        <v>41757</v>
+    <row r="11" spans="1:86" ht="63" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B11" s="24" t="s">
         <v>570</v>
@@ -6351,9 +6366,9 @@
         <v>413</v>
       </c>
     </row>
-    <row r="12" spans="1:86" ht="31.5">
-      <c r="A12" s="22">
-        <v>41757</v>
+    <row r="12" spans="1:86" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B12" s="24" t="s">
         <v>571</v>
@@ -6380,9 +6395,9 @@
         <v>411</v>
       </c>
     </row>
-    <row r="13" spans="1:86" s="3" customFormat="1" ht="31.5">
-      <c r="A13" s="22">
-        <v>41757</v>
+    <row r="13" spans="1:86" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B13" s="24" t="s">
         <v>572</v>
@@ -6409,9 +6424,9 @@
         <v>409</v>
       </c>
     </row>
-    <row r="14" spans="1:86" s="3" customFormat="1" ht="31.5">
-      <c r="A14" s="22">
-        <v>41757</v>
+    <row r="14" spans="1:86" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B14" s="24" t="s">
         <v>573</v>
@@ -6438,9 +6453,9 @@
         <v>407</v>
       </c>
     </row>
-    <row r="15" spans="1:86" s="3" customFormat="1" ht="31.5">
-      <c r="A15" s="22">
-        <v>41757</v>
+    <row r="15" spans="1:86" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B15" s="24" t="s">
         <v>574</v>
@@ -6467,9 +6482,9 @@
         <v>405</v>
       </c>
     </row>
-    <row r="16" spans="1:86" s="3" customFormat="1" ht="31.5">
-      <c r="A16" s="22">
-        <v>41757</v>
+    <row r="16" spans="1:86" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B16" s="24" t="s">
         <v>575</v>
@@ -6496,9 +6511,9 @@
         <v>403</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="3" customFormat="1" ht="47.25">
-      <c r="A17" s="22">
-        <v>41757</v>
+    <row r="17" spans="1:11" s="3" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B17" s="24" t="s">
         <v>576</v>
@@ -6525,9 +6540,9 @@
         <v>401</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="3" customFormat="1" ht="31.5">
-      <c r="A18" s="22">
-        <v>41757</v>
+    <row r="18" spans="1:11" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B18" s="24" t="s">
         <v>577</v>
@@ -6554,9 +6569,9 @@
         <v>399</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="3" customFormat="1" ht="31.5">
-      <c r="A19" s="22">
-        <v>41757</v>
+    <row r="19" spans="1:11" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B19" s="24" t="s">
         <v>578</v>
@@ -6583,9 +6598,9 @@
         <v>397</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="3" customFormat="1" ht="31.5">
-      <c r="A20" s="22">
-        <v>41757</v>
+    <row r="20" spans="1:11" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B20" s="24" t="s">
         <v>579</v>
@@ -6612,9 +6627,9 @@
         <v>395</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="3" customFormat="1" ht="31.5">
-      <c r="A21" s="22">
-        <v>41757</v>
+    <row r="21" spans="1:11" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B21" s="24" t="s">
         <v>580</v>
@@ -6641,9 +6656,9 @@
         <v>393</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="3" customFormat="1" ht="31.5">
-      <c r="A22" s="22">
-        <v>41757</v>
+    <row r="22" spans="1:11" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B22" s="24" t="s">
         <v>581</v>
@@ -6670,9 +6685,9 @@
         <v>391</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="31.5">
-      <c r="A23" s="22">
-        <v>41757</v>
+    <row r="23" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B23" s="24" t="s">
         <v>582</v>
@@ -6699,9 +6714,9 @@
         <v>389</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="31.5">
-      <c r="A24" s="22">
-        <v>41757</v>
+    <row r="24" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B24" s="24" t="s">
         <v>583</v>
@@ -6728,9 +6743,9 @@
         <v>387</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="31.5">
-      <c r="A25" s="22">
-        <v>41757</v>
+    <row r="25" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B25" s="24" t="s">
         <v>584</v>
@@ -6757,9 +6772,9 @@
         <v>382</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="47.25">
-      <c r="A26" s="22">
-        <v>41757</v>
+    <row r="26" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B26" s="24" t="s">
         <v>585</v>
@@ -6786,9 +6801,9 @@
         <v>379</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="31.5">
-      <c r="A27" s="22">
-        <v>41757</v>
+    <row r="27" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B27" s="24" t="s">
         <v>586</v>
@@ -6815,9 +6830,9 @@
         <v>376</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="31.5">
-      <c r="A28" s="22">
-        <v>41757</v>
+    <row r="28" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B28" s="24" t="s">
         <v>587</v>
@@ -6844,9 +6859,9 @@
         <v>372</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="31.5">
-      <c r="A29" s="22">
-        <v>41757</v>
+    <row r="29" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B29" s="24" t="s">
         <v>588</v>
@@ -6873,9 +6888,9 @@
         <v>371</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="47.25">
-      <c r="A30" s="22">
-        <v>41757</v>
+    <row r="30" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A30" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B30" s="24" t="s">
         <v>589</v>
@@ -6902,9 +6917,9 @@
         <v>368</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="31.5">
-      <c r="A31" s="22">
-        <v>41757</v>
+    <row r="31" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A31" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B31" s="24" t="s">
         <v>590</v>
@@ -6931,9 +6946,9 @@
         <v>365</v>
       </c>
     </row>
-    <row r="32" spans="1:11" s="3" customFormat="1" ht="47.25">
-      <c r="A32" s="22">
-        <v>41757</v>
+    <row r="32" spans="1:11" s="3" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A32" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B32" s="24" t="s">
         <v>591</v>
@@ -6960,9 +6975,9 @@
         <v>361</v>
       </c>
     </row>
-    <row r="33" spans="1:11" s="3" customFormat="1" ht="63">
-      <c r="A33" s="22">
-        <v>41757</v>
+    <row r="33" spans="1:11" s="3" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A33" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B33" s="24" t="s">
         <v>592</v>
@@ -6989,9 +7004,9 @@
         <v>360</v>
       </c>
     </row>
-    <row r="34" spans="1:11" s="3" customFormat="1" ht="78.75">
-      <c r="A34" s="22">
-        <v>41757</v>
+    <row r="34" spans="1:11" s="3" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B34" s="24" t="s">
         <v>593</v>
@@ -7018,9 +7033,9 @@
         <v>359</v>
       </c>
     </row>
-    <row r="35" spans="1:11" s="3" customFormat="1" ht="63">
-      <c r="A35" s="22">
-        <v>41757</v>
+    <row r="35" spans="1:11" s="3" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A35" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B35" s="24" t="s">
         <v>594</v>
@@ -7047,9 +7062,9 @@
         <v>355</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="63">
-      <c r="A36" s="22">
-        <v>41757</v>
+    <row r="36" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A36" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B36" s="24" t="s">
         <v>595</v>
@@ -7076,9 +7091,9 @@
         <v>351</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="78.75">
-      <c r="A37" s="22">
-        <v>41757</v>
+    <row r="37" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B37" s="24" t="s">
         <v>596</v>
@@ -7105,9 +7120,9 @@
         <v>347</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="126">
-      <c r="A38" s="22">
-        <v>41757</v>
+    <row r="38" spans="1:11" ht="126" x14ac:dyDescent="0.25">
+      <c r="A38" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B38" s="24" t="s">
         <v>597</v>
@@ -7134,9 +7149,9 @@
         <v>343</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="63">
-      <c r="A39" s="22">
-        <v>41757</v>
+    <row r="39" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A39" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B39" s="24" t="s">
         <v>598</v>
@@ -7163,9 +7178,9 @@
         <v>341</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="63">
-      <c r="A40" s="22">
-        <v>41757</v>
+    <row r="40" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A40" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B40" s="24" t="s">
         <v>599</v>
@@ -7192,9 +7207,9 @@
         <v>339</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="63">
-      <c r="A41" s="22">
-        <v>41757</v>
+    <row r="41" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A41" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B41" s="24" t="s">
         <v>600</v>
@@ -7221,9 +7236,9 @@
         <v>335</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="78.75">
-      <c r="A42" s="22">
-        <v>41757</v>
+    <row r="42" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B42" s="24" t="s">
         <v>601</v>
@@ -7250,9 +7265,9 @@
         <v>330</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="220.5">
-      <c r="A43" s="22">
-        <v>41757</v>
+    <row r="43" spans="1:11" ht="220.5" x14ac:dyDescent="0.25">
+      <c r="A43" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B43" s="24" t="s">
         <v>602</v>
@@ -7279,9 +7294,9 @@
         <v>552</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="220.5">
-      <c r="A44" s="22">
-        <v>41757</v>
+    <row r="44" spans="1:11" ht="220.5" x14ac:dyDescent="0.25">
+      <c r="A44" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B44" s="24" t="s">
         <v>603</v>
@@ -7308,9 +7323,9 @@
         <v>554</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="252">
-      <c r="A45" s="22">
-        <v>41757</v>
+    <row r="45" spans="1:11" ht="252" x14ac:dyDescent="0.25">
+      <c r="A45" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B45" s="24" t="s">
         <v>604</v>
@@ -7337,9 +7352,9 @@
         <v>556</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="63">
-      <c r="A46" s="22">
-        <v>41757</v>
+    <row r="46" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A46" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B46" s="24" t="s">
         <v>605</v>
@@ -7366,9 +7381,9 @@
         <v>323</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="78.75">
-      <c r="A47" s="22">
-        <v>41757</v>
+    <row r="47" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B47" s="24" t="s">
         <v>606</v>
@@ -7392,9 +7407,9 @@
         <v>319</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="94.5">
-      <c r="A48" s="22">
-        <v>41757</v>
+    <row r="48" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A48" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B48" s="24" t="s">
         <v>607</v>
@@ -7421,9 +7436,9 @@
         <v>317</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="94.5">
-      <c r="A49" s="22">
-        <v>41757</v>
+    <row r="49" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A49" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B49" s="24" t="s">
         <v>608</v>
@@ -7450,9 +7465,9 @@
         <v>315</v>
       </c>
     </row>
-    <row r="50" spans="1:11" s="3" customFormat="1" ht="94.5">
-      <c r="A50" s="22">
-        <v>41757</v>
+    <row r="50" spans="1:11" s="3" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A50" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B50" s="26" t="s">
         <v>609</v>
@@ -7479,9 +7494,9 @@
         <v>313</v>
       </c>
     </row>
-    <row r="51" spans="1:11" s="3" customFormat="1" ht="94.5">
-      <c r="A51" s="22">
-        <v>41757</v>
+    <row r="51" spans="1:11" s="3" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A51" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B51" s="24" t="s">
         <v>610</v>
@@ -7508,9 +7523,9 @@
         <v>311</v>
       </c>
     </row>
-    <row r="52" spans="1:11" s="3" customFormat="1" ht="94.5">
-      <c r="A52" s="22">
-        <v>41757</v>
+    <row r="52" spans="1:11" s="3" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A52" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B52" s="24" t="s">
         <v>611</v>
@@ -7537,9 +7552,9 @@
         <v>309</v>
       </c>
     </row>
-    <row r="53" spans="1:11" s="3" customFormat="1" ht="94.5">
-      <c r="A53" s="22">
-        <v>41757</v>
+    <row r="53" spans="1:11" s="3" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A53" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B53" s="24" t="s">
         <v>612</v>
@@ -7566,9 +7581,9 @@
         <v>307</v>
       </c>
     </row>
-    <row r="54" spans="1:11" s="3" customFormat="1" ht="94.5">
-      <c r="A54" s="22">
-        <v>41757</v>
+    <row r="54" spans="1:11" s="3" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A54" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B54" s="24" t="s">
         <v>613</v>
@@ -7595,9 +7610,9 @@
         <v>305</v>
       </c>
     </row>
-    <row r="55" spans="1:11" s="3" customFormat="1" ht="94.5">
-      <c r="A55" s="22">
-        <v>41757</v>
+    <row r="55" spans="1:11" s="3" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A55" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B55" s="24" t="s">
         <v>614</v>
@@ -7624,9 +7639,9 @@
         <v>300</v>
       </c>
     </row>
-    <row r="56" spans="1:11" s="3" customFormat="1" ht="98.45" customHeight="1">
-      <c r="A56" s="22">
-        <v>41757</v>
+    <row r="56" spans="1:11" s="3" customFormat="1" ht="98.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B56" s="26" t="s">
         <v>615</v>
@@ -7655,9 +7670,9 @@
         <v>476</v>
       </c>
     </row>
-    <row r="57" spans="1:11" s="3" customFormat="1" ht="94.5">
-      <c r="A57" s="22">
-        <v>41757</v>
+    <row r="57" spans="1:11" s="3" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A57" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B57" s="24" t="s">
         <v>616</v>
@@ -7684,9 +7699,9 @@
         <v>297</v>
       </c>
     </row>
-    <row r="58" spans="1:11" s="3" customFormat="1" ht="94.5">
-      <c r="A58" s="22">
-        <v>41757</v>
+    <row r="58" spans="1:11" s="3" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A58" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B58" s="24" t="s">
         <v>617</v>
@@ -7713,9 +7728,9 @@
         <v>294</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="94.5">
-      <c r="A59" s="22">
-        <v>41757</v>
+    <row r="59" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A59" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B59" s="24" t="s">
         <v>618</v>
@@ -7742,9 +7757,9 @@
         <v>291</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="94.5">
-      <c r="A60" s="22">
-        <v>41757</v>
+    <row r="60" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A60" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B60" s="24" t="s">
         <v>619</v>
@@ -7771,9 +7786,9 @@
         <v>288</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="94.5">
-      <c r="A61" s="22">
-        <v>41757</v>
+    <row r="61" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A61" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B61" s="24" t="s">
         <v>620</v>
@@ -7800,9 +7815,9 @@
         <v>285</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="94.5">
-      <c r="A62" s="22">
-        <v>41757</v>
+    <row r="62" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A62" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B62" s="24" t="s">
         <v>621</v>
@@ -7829,9 +7844,9 @@
         <v>283</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="31.5">
-      <c r="A63" s="22">
-        <v>41757</v>
+    <row r="63" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A63" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B63" s="24" t="s">
         <v>622</v>
@@ -7858,9 +7873,9 @@
         <v>281</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="110.25">
-      <c r="A64" s="22">
-        <v>41757</v>
+    <row r="64" spans="1:11" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A64" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B64" s="24" t="s">
         <v>623</v>
@@ -7887,9 +7902,9 @@
         <v>279</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="94.5">
-      <c r="A65" s="22">
-        <v>41757</v>
+    <row r="65" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A65" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B65" s="24" t="s">
         <v>624</v>
@@ -7916,9 +7931,9 @@
         <v>277</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="94.5">
-      <c r="A66" s="22">
-        <v>41757</v>
+    <row r="66" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A66" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B66" s="24" t="s">
         <v>625</v>
@@ -7945,9 +7960,9 @@
         <v>274</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="110.25">
-      <c r="A67" s="22">
-        <v>41757</v>
+    <row r="67" spans="1:11" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A67" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B67" s="24" t="s">
         <v>626</v>
@@ -7974,9 +7989,9 @@
         <v>271</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="94.5">
-      <c r="A68" s="22">
-        <v>41757</v>
+    <row r="68" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A68" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B68" s="24" t="s">
         <v>627</v>
@@ -8003,9 +8018,9 @@
         <v>269</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="94.5">
-      <c r="A69" s="22">
-        <v>41757</v>
+    <row r="69" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A69" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B69" s="24" t="s">
         <v>628</v>
@@ -8032,9 +8047,9 @@
         <v>265</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="31.5">
-      <c r="A70" s="22">
-        <v>41757</v>
+    <row r="70" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A70" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B70" s="24" t="s">
         <v>629</v>
@@ -8061,9 +8076,9 @@
         <v>263</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="31.5">
-      <c r="A71" s="22">
-        <v>41757</v>
+    <row r="71" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A71" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B71" s="24" t="s">
         <v>630</v>
@@ -8090,9 +8105,9 @@
         <v>261</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="31.5">
-      <c r="A72" s="22">
-        <v>41757</v>
+    <row r="72" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A72" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B72" s="24" t="s">
         <v>631</v>
@@ -8119,9 +8134,9 @@
         <v>256</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="94.5">
-      <c r="A73" s="22">
-        <v>41757</v>
+    <row r="73" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A73" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B73" s="24" t="s">
         <v>632</v>
@@ -8148,9 +8163,9 @@
         <v>254</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="94.5">
-      <c r="A74" s="22">
-        <v>41757</v>
+    <row r="74" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A74" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B74" s="24" t="s">
         <v>633</v>
@@ -8177,9 +8192,9 @@
         <v>252</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="94.5">
-      <c r="A75" s="22">
-        <v>41757</v>
+    <row r="75" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A75" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B75" s="24" t="s">
         <v>634</v>
@@ -8206,9 +8221,9 @@
         <v>250</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="94.5">
-      <c r="A76" s="22">
-        <v>41757</v>
+    <row r="76" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A76" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B76" s="24" t="s">
         <v>635</v>
@@ -8235,9 +8250,9 @@
         <v>248</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="94.5">
-      <c r="A77" s="22">
-        <v>41757</v>
+    <row r="77" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A77" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B77" s="24" t="s">
         <v>636</v>
@@ -8264,9 +8279,9 @@
         <v>246</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="94.5">
-      <c r="A78" s="22">
-        <v>41757</v>
+    <row r="78" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A78" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B78" s="24" t="s">
         <v>637</v>
@@ -8293,9 +8308,9 @@
         <v>241</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="63">
-      <c r="A79" s="22">
-        <v>41757</v>
+    <row r="79" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A79" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B79" s="24" t="s">
         <v>638</v>
@@ -8326,9 +8341,9 @@
         <v>239</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="63">
-      <c r="A80" s="22">
-        <v>41757</v>
+    <row r="80" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A80" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B80" s="24" t="s">
         <v>639</v>
@@ -8359,9 +8374,9 @@
         <v>237</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="63">
-      <c r="A81" s="22">
-        <v>41757</v>
+    <row r="81" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A81" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B81" s="26" t="s">
         <v>640</v>
@@ -8392,9 +8407,9 @@
         <v>235</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="63">
-      <c r="A82" s="22">
-        <v>41757</v>
+    <row r="82" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A82" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B82" s="24" t="s">
         <v>641</v>
@@ -8425,9 +8440,9 @@
         <v>233</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="63">
-      <c r="A83" s="22">
-        <v>41757</v>
+    <row r="83" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A83" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B83" s="24" t="s">
         <v>642</v>
@@ -8458,9 +8473,9 @@
         <v>231</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="78.75">
-      <c r="A84" s="22">
-        <v>41757</v>
+    <row r="84" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A84" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B84" s="24" t="s">
         <v>643</v>
@@ -8491,9 +8506,9 @@
         <v>229</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="63">
-      <c r="A85" s="22">
-        <v>41757</v>
+    <row r="85" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A85" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B85" s="24" t="s">
         <v>644</v>
@@ -8524,9 +8539,9 @@
         <v>227</v>
       </c>
     </row>
-    <row r="86" spans="1:11" ht="63">
-      <c r="A86" s="22">
-        <v>41757</v>
+    <row r="86" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A86" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B86" s="24" t="s">
         <v>645</v>
@@ -8557,9 +8572,9 @@
         <v>225</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="78.75">
-      <c r="A87" s="22">
-        <v>41757</v>
+    <row r="87" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A87" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B87" s="24" t="s">
         <v>646</v>
@@ -8590,9 +8605,9 @@
         <v>222</v>
       </c>
     </row>
-    <row r="88" spans="1:11" ht="63">
-      <c r="A88" s="22">
-        <v>41757</v>
+    <row r="88" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A88" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B88" s="24" t="s">
         <v>647</v>
@@ -8619,9 +8634,9 @@
         <v>220</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="63">
-      <c r="A89" s="22">
-        <v>41757</v>
+    <row r="89" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A89" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B89" s="24" t="s">
         <v>648</v>
@@ -8652,9 +8667,9 @@
         <v>217</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="63">
-      <c r="A90" s="22">
-        <v>41757</v>
+    <row r="90" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A90" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B90" s="24" t="s">
         <v>649</v>
@@ -8681,9 +8696,9 @@
         <v>215</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="94.5">
-      <c r="A91" s="22">
-        <v>41757</v>
+    <row r="91" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A91" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B91" s="24" t="s">
         <v>650</v>
@@ -8712,9 +8727,9 @@
         <v>213</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="94.5">
-      <c r="A92" s="22">
-        <v>41757</v>
+    <row r="92" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A92" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B92" s="24" t="s">
         <v>651</v>
@@ -8743,9 +8758,9 @@
         <v>210</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="63">
-      <c r="A93" s="22">
-        <v>41757</v>
+    <row r="93" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A93" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B93" s="24" t="s">
         <v>652</v>
@@ -8776,9 +8791,9 @@
         <v>208</v>
       </c>
     </row>
-    <row r="94" spans="1:11" ht="94.5">
-      <c r="A94" s="22">
-        <v>41757</v>
+    <row r="94" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A94" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B94" s="24" t="s">
         <v>653</v>
@@ -8809,9 +8824,9 @@
         <v>205</v>
       </c>
     </row>
-    <row r="95" spans="1:11" ht="63">
-      <c r="A95" s="22">
-        <v>41757</v>
+    <row r="95" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A95" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B95" s="24" t="s">
         <v>654</v>
@@ -8842,9 +8857,9 @@
         <v>203</v>
       </c>
     </row>
-    <row r="96" spans="1:11" ht="63">
-      <c r="A96" s="22">
-        <v>41757</v>
+    <row r="96" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A96" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B96" s="24" t="s">
         <v>655</v>
@@ -8875,9 +8890,9 @@
         <v>201</v>
       </c>
     </row>
-    <row r="97" spans="1:11" ht="63">
-      <c r="A97" s="22">
-        <v>41757</v>
+    <row r="97" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A97" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B97" s="24" t="s">
         <v>656</v>
@@ -8904,9 +8919,9 @@
         <v>199</v>
       </c>
     </row>
-    <row r="98" spans="1:11" ht="63">
-      <c r="A98" s="22">
-        <v>41757</v>
+    <row r="98" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A98" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B98" s="24" t="s">
         <v>657</v>
@@ -8937,9 +8952,9 @@
         <v>197</v>
       </c>
     </row>
-    <row r="99" spans="1:11" ht="63">
-      <c r="A99" s="22">
-        <v>41757</v>
+    <row r="99" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A99" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B99" s="24" t="s">
         <v>658</v>
@@ -8966,9 +8981,9 @@
         <v>195</v>
       </c>
     </row>
-    <row r="100" spans="1:11" ht="63">
-      <c r="A100" s="22">
-        <v>41757</v>
+    <row r="100" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A100" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B100" s="24" t="s">
         <v>659</v>
@@ -8999,9 +9014,9 @@
         <v>193</v>
       </c>
     </row>
-    <row r="101" spans="1:11" ht="63">
-      <c r="A101" s="22">
-        <v>41757</v>
+    <row r="101" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A101" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B101" s="24" t="s">
         <v>660</v>
@@ -9032,9 +9047,9 @@
         <v>191</v>
       </c>
     </row>
-    <row r="102" spans="1:11" ht="63">
-      <c r="A102" s="22">
-        <v>41757</v>
+    <row r="102" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A102" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B102" s="24" t="s">
         <v>661</v>
@@ -9065,9 +9080,9 @@
         <v>189</v>
       </c>
     </row>
-    <row r="103" spans="1:11" ht="63">
-      <c r="A103" s="22">
-        <v>41757</v>
+    <row r="103" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A103" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B103" s="24" t="s">
         <v>662</v>
@@ -9098,9 +9113,9 @@
         <v>187</v>
       </c>
     </row>
-    <row r="104" spans="1:11" ht="63">
-      <c r="A104" s="22">
-        <v>41757</v>
+    <row r="104" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A104" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B104" s="24" t="s">
         <v>663</v>
@@ -9131,9 +9146,9 @@
         <v>185</v>
       </c>
     </row>
-    <row r="105" spans="1:11" ht="63">
-      <c r="A105" s="22">
-        <v>41757</v>
+    <row r="105" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A105" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B105" s="24" t="s">
         <v>664</v>
@@ -9164,9 +9179,9 @@
         <v>183</v>
       </c>
     </row>
-    <row r="106" spans="1:11" ht="63">
-      <c r="A106" s="22">
-        <v>41757</v>
+    <row r="106" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A106" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B106" s="24" t="s">
         <v>665</v>
@@ -9197,9 +9212,9 @@
         <v>181</v>
       </c>
     </row>
-    <row r="107" spans="1:11" ht="63">
-      <c r="A107" s="22">
-        <v>41757</v>
+    <row r="107" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A107" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B107" s="24" t="s">
         <v>666</v>
@@ -9226,9 +9241,9 @@
         <v>178</v>
       </c>
     </row>
-    <row r="108" spans="1:11" ht="78.75">
-      <c r="A108" s="22">
-        <v>41757</v>
+    <row r="108" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A108" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B108" s="24" t="s">
         <v>667</v>
@@ -9259,9 +9274,9 @@
         <v>176</v>
       </c>
     </row>
-    <row r="109" spans="1:11" ht="63">
-      <c r="A109" s="22">
-        <v>41757</v>
+    <row r="109" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A109" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B109" s="24" t="s">
         <v>668</v>
@@ -9292,9 +9307,9 @@
         <v>174</v>
       </c>
     </row>
-    <row r="110" spans="1:11" ht="110.25">
-      <c r="A110" s="22">
-        <v>41757</v>
+    <row r="110" spans="1:11" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A110" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B110" s="24" t="s">
         <v>669</v>
@@ -9325,9 +9340,9 @@
         <v>171</v>
       </c>
     </row>
-    <row r="111" spans="1:11" ht="63">
-      <c r="A111" s="22">
-        <v>41757</v>
+    <row r="111" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A111" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B111" s="24" t="s">
         <v>670</v>
@@ -9358,9 +9373,9 @@
         <v>167</v>
       </c>
     </row>
-    <row r="112" spans="1:11" ht="63">
-      <c r="A112" s="22">
-        <v>41757</v>
+    <row r="112" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A112" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B112" s="24" t="s">
         <v>671</v>
@@ -9387,9 +9402,9 @@
         <v>165</v>
       </c>
     </row>
-    <row r="113" spans="1:11" ht="63">
-      <c r="A113" s="22">
-        <v>41757</v>
+    <row r="113" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A113" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B113" s="24" t="s">
         <v>672</v>
@@ -9416,9 +9431,9 @@
         <v>161</v>
       </c>
     </row>
-    <row r="114" spans="1:11" ht="126">
-      <c r="A114" s="22">
-        <v>41757</v>
+    <row r="114" spans="1:11" ht="126" x14ac:dyDescent="0.25">
+      <c r="A114" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B114" s="24" t="s">
         <v>673</v>
@@ -9447,9 +9462,9 @@
         <v>159</v>
       </c>
     </row>
-    <row r="115" spans="1:11" ht="110.25">
-      <c r="A115" s="22">
-        <v>41757</v>
+    <row r="115" spans="1:11" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A115" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B115" s="24" t="s">
         <v>674</v>
@@ -9480,9 +9495,9 @@
         <v>157</v>
       </c>
     </row>
-    <row r="116" spans="1:11" ht="94.5">
-      <c r="A116" s="22">
-        <v>41757</v>
+    <row r="116" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A116" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B116" s="24" t="s">
         <v>675</v>
@@ -9513,9 +9528,9 @@
         <v>155</v>
       </c>
     </row>
-    <row r="117" spans="1:11" ht="94.5">
-      <c r="A117" s="22">
-        <v>41757</v>
+    <row r="117" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A117" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B117" s="24" t="s">
         <v>676</v>
@@ -9546,9 +9561,9 @@
         <v>152</v>
       </c>
     </row>
-    <row r="118" spans="1:11" ht="220.5">
-      <c r="A118" s="22">
-        <v>41757</v>
+    <row r="118" spans="1:11" ht="220.5" x14ac:dyDescent="0.25">
+      <c r="A118" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B118" s="24" t="s">
         <v>677</v>
@@ -9575,9 +9590,9 @@
         <v>147</v>
       </c>
     </row>
-    <row r="119" spans="1:11" ht="47.25">
-      <c r="A119" s="22">
-        <v>41757</v>
+    <row r="119" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A119" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B119" s="24" t="s">
         <v>678</v>
@@ -9604,9 +9619,9 @@
         <v>143</v>
       </c>
     </row>
-    <row r="120" spans="1:11" ht="63">
-      <c r="A120" s="22">
-        <v>41757</v>
+    <row r="120" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A120" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B120" s="24" t="s">
         <v>679</v>
@@ -9633,9 +9648,9 @@
         <v>138</v>
       </c>
     </row>
-    <row r="121" spans="1:11" ht="294.75" customHeight="1">
-      <c r="A121" s="23">
-        <v>41764</v>
+    <row r="121" spans="1:11" ht="294.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="23" t="d">
+        <v>2014-05-05</v>
       </c>
       <c r="B121" s="26" t="s">
         <v>680</v>
@@ -9668,9 +9683,9 @@
         <v>839</v>
       </c>
     </row>
-    <row r="122" spans="1:11" ht="126">
-      <c r="A122" s="22">
-        <v>41757</v>
+    <row r="122" spans="1:11" ht="126" x14ac:dyDescent="0.25">
+      <c r="A122" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B122" s="24" t="s">
         <v>681</v>
@@ -9701,9 +9716,9 @@
         <v>135</v>
       </c>
     </row>
-    <row r="123" spans="1:11" ht="126">
-      <c r="A123" s="22">
-        <v>41757</v>
+    <row r="123" spans="1:11" ht="126" x14ac:dyDescent="0.25">
+      <c r="A123" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B123" s="24" t="s">
         <v>682</v>
@@ -9732,9 +9747,9 @@
         <v>131</v>
       </c>
     </row>
-    <row r="124" spans="1:11" ht="63">
-      <c r="A124" s="22">
-        <v>41757</v>
+    <row r="124" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A124" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B124" s="24" t="s">
         <v>683</v>
@@ -9761,9 +9776,9 @@
         <v>127</v>
       </c>
     </row>
-    <row r="125" spans="1:11" ht="63">
-      <c r="A125" s="22">
-        <v>41757</v>
+    <row r="125" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A125" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B125" s="24" t="s">
         <v>684</v>
@@ -9790,9 +9805,9 @@
         <v>138</v>
       </c>
     </row>
-    <row r="126" spans="1:11" ht="204.75">
-      <c r="A126" s="22">
-        <v>41757</v>
+    <row r="126" spans="1:11" ht="204.75" x14ac:dyDescent="0.25">
+      <c r="A126" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B126" s="24" t="s">
         <v>685</v>
@@ -9823,9 +9838,9 @@
         <v>123</v>
       </c>
     </row>
-    <row r="127" spans="1:11" ht="157.5">
-      <c r="A127" s="22">
-        <v>41757</v>
+    <row r="127" spans="1:11" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A127" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B127" s="24" t="s">
         <v>686</v>
@@ -9856,9 +9871,9 @@
         <v>121</v>
       </c>
     </row>
-    <row r="128" spans="1:11" ht="47.25">
-      <c r="A128" s="22">
-        <v>41757</v>
+    <row r="128" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A128" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B128" s="24" t="s">
         <v>687</v>
@@ -9889,9 +9904,9 @@
         <v>119</v>
       </c>
     </row>
-    <row r="129" spans="1:11" ht="94.5">
-      <c r="A129" s="22">
-        <v>41757</v>
+    <row r="129" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A129" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B129" s="24" t="s">
         <v>688</v>
@@ -9922,9 +9937,9 @@
         <v>116</v>
       </c>
     </row>
-    <row r="130" spans="1:11" s="1" customFormat="1" ht="78.75">
-      <c r="A130" s="22">
-        <v>41757</v>
+    <row r="130" spans="1:11" s="1" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A130" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B130" s="24" t="s">
         <v>689</v>
@@ -9953,9 +9968,9 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="131" spans="1:11" ht="63">
-      <c r="A131" s="22">
-        <v>41757</v>
+    <row r="131" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A131" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B131" s="24" t="s">
         <v>690</v>
@@ -9986,9 +10001,9 @@
         <v>112</v>
       </c>
     </row>
-    <row r="132" spans="1:11" ht="63">
-      <c r="A132" s="22">
-        <v>41757</v>
+    <row r="132" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A132" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B132" s="24" t="s">
         <v>691</v>
@@ -10019,9 +10034,9 @@
         <v>110</v>
       </c>
     </row>
-    <row r="133" spans="1:11" ht="94.5">
-      <c r="A133" s="22">
-        <v>41757</v>
+    <row r="133" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A133" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B133" s="24" t="s">
         <v>692</v>
@@ -10052,9 +10067,9 @@
         <v>106</v>
       </c>
     </row>
-    <row r="134" spans="1:11" ht="133.5" customHeight="1">
-      <c r="A134" s="22">
-        <v>41757</v>
+    <row r="134" spans="1:11" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B134" s="24" t="s">
         <v>693</v>
@@ -10085,9 +10100,9 @@
         <v>104</v>
       </c>
     </row>
-    <row r="135" spans="1:11" ht="157.5">
-      <c r="A135" s="22">
-        <v>41757</v>
+    <row r="135" spans="1:11" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A135" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B135" s="24" t="s">
         <v>694</v>
@@ -10118,9 +10133,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="136" spans="1:11" ht="110.25">
-      <c r="A136" s="22">
-        <v>41757</v>
+    <row r="136" spans="1:11" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A136" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B136" s="24" t="s">
         <v>695</v>
@@ -10147,9 +10162,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="137" spans="1:11" ht="94.5">
-      <c r="A137" s="22">
-        <v>41757</v>
+    <row r="137" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A137" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B137" s="24" t="s">
         <v>696</v>
@@ -10176,9 +10191,9 @@
         <v>98</v>
       </c>
     </row>
-    <row r="138" spans="1:11" ht="126">
-      <c r="A138" s="22">
-        <v>41757</v>
+    <row r="138" spans="1:11" ht="126" x14ac:dyDescent="0.25">
+      <c r="A138" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B138" s="24" t="s">
         <v>697</v>
@@ -10205,9 +10220,9 @@
         <v>96</v>
       </c>
     </row>
-    <row r="139" spans="1:11" ht="110.25">
-      <c r="A139" s="22">
-        <v>41757</v>
+    <row r="139" spans="1:11" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A139" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B139" s="24" t="s">
         <v>698</v>
@@ -10234,9 +10249,9 @@
         <v>94</v>
       </c>
     </row>
-    <row r="140" spans="1:11" ht="110.25">
-      <c r="A140" s="22">
-        <v>41757</v>
+    <row r="140" spans="1:11" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A140" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B140" s="24" t="s">
         <v>699</v>
@@ -10263,9 +10278,9 @@
         <v>92</v>
       </c>
     </row>
-    <row r="141" spans="1:11" ht="110.25">
-      <c r="A141" s="22">
-        <v>41757</v>
+    <row r="141" spans="1:11" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A141" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B141" s="24" t="s">
         <v>700</v>
@@ -10292,9 +10307,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="142" spans="1:11" ht="141.75">
-      <c r="A142" s="22">
-        <v>41757</v>
+    <row r="142" spans="1:11" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="A142" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B142" s="24" t="s">
         <v>701</v>
@@ -10321,9 +10336,9 @@
         <v>88</v>
       </c>
     </row>
-    <row r="143" spans="1:11" ht="126">
-      <c r="A143" s="22">
-        <v>41757</v>
+    <row r="143" spans="1:11" ht="126" x14ac:dyDescent="0.25">
+      <c r="A143" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B143" s="24" t="s">
         <v>702</v>
@@ -10350,9 +10365,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="144" spans="1:11" ht="157.5">
-      <c r="A144" s="22">
-        <v>41757</v>
+    <row r="144" spans="1:11" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A144" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B144" s="24" t="s">
         <v>703</v>
@@ -10383,9 +10398,9 @@
         <v>83</v>
       </c>
     </row>
-    <row r="145" spans="1:11" ht="94.5">
-      <c r="A145" s="22">
-        <v>41757</v>
+    <row r="145" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A145" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B145" s="24" t="s">
         <v>704</v>
@@ -10412,9 +10427,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="146" spans="1:11" ht="47.25">
-      <c r="A146" s="22">
-        <v>41757</v>
+    <row r="146" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A146" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B146" s="24" t="s">
         <v>705</v>
@@ -10445,9 +10460,9 @@
         <v>75</v>
       </c>
     </row>
-    <row r="147" spans="1:11" ht="141.75">
-      <c r="A147" s="22">
-        <v>41757</v>
+    <row r="147" spans="1:11" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="A147" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B147" s="24" t="s">
         <v>706</v>
@@ -10478,9 +10493,9 @@
         <v>73</v>
       </c>
     </row>
-    <row r="148" spans="1:11" ht="31.5">
-      <c r="A148" s="22">
-        <v>41757</v>
+    <row r="148" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A148" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B148" s="24" t="s">
         <v>707</v>
@@ -10511,9 +10526,9 @@
         <v>71</v>
       </c>
     </row>
-    <row r="149" spans="1:11" ht="47.25">
-      <c r="A149" s="22">
-        <v>41757</v>
+    <row r="149" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A149" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B149" s="24" t="s">
         <v>708</v>
@@ -10544,9 +10559,9 @@
         <v>69</v>
       </c>
     </row>
-    <row r="150" spans="1:11" ht="78.75">
-      <c r="A150" s="22">
-        <v>41757</v>
+    <row r="150" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A150" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B150" s="24" t="s">
         <v>709</v>
@@ -10577,9 +10592,9 @@
         <v>68</v>
       </c>
     </row>
-    <row r="151" spans="1:11" ht="141.75">
-      <c r="A151" s="22">
-        <v>41757</v>
+    <row r="151" spans="1:11" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="A151" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B151" s="24" t="s">
         <v>710</v>
@@ -10610,9 +10625,9 @@
         <v>66</v>
       </c>
     </row>
-    <row r="152" spans="1:11" ht="157.5">
-      <c r="A152" s="22">
-        <v>41757</v>
+    <row r="152" spans="1:11" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A152" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B152" s="24" t="s">
         <v>711</v>
@@ -10643,9 +10658,9 @@
         <v>64</v>
       </c>
     </row>
-    <row r="153" spans="1:11" ht="78.75">
-      <c r="A153" s="22">
-        <v>41757</v>
+    <row r="153" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A153" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B153" s="24" t="s">
         <v>712</v>
@@ -10676,9 +10691,9 @@
         <v>62</v>
       </c>
     </row>
-    <row r="154" spans="1:11" ht="157.5">
-      <c r="A154" s="22">
-        <v>41757</v>
+    <row r="154" spans="1:11" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A154" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B154" s="24" t="s">
         <v>713</v>
@@ -10709,9 +10724,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="155" spans="1:11" ht="231" customHeight="1">
-      <c r="A155" s="22">
-        <v>41757</v>
+    <row r="155" spans="1:11" ht="231" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B155" s="24" t="s">
         <v>714</v>
@@ -10742,9 +10757,9 @@
         <v>58</v>
       </c>
     </row>
-    <row r="156" spans="1:11" ht="243.75" customHeight="1">
-      <c r="A156" s="22">
-        <v>41757</v>
+    <row r="156" spans="1:11" ht="243.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B156" s="24" t="s">
         <v>715</v>
@@ -10775,9 +10790,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="157" spans="1:11" ht="47.25">
-      <c r="A157" s="22">
-        <v>41757</v>
+    <row r="157" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A157" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B157" s="24" t="s">
         <v>716</v>
@@ -10808,9 +10823,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="158" spans="1:11" ht="110.25">
-      <c r="A158" s="22">
-        <v>41757</v>
+    <row r="158" spans="1:11" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A158" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B158" s="24" t="s">
         <v>717</v>
@@ -10841,9 +10856,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="159" spans="1:11" ht="126">
-      <c r="A159" s="22">
-        <v>41757</v>
+    <row r="159" spans="1:11" ht="126" x14ac:dyDescent="0.25">
+      <c r="A159" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B159" s="24" t="s">
         <v>718</v>
@@ -10874,9 +10889,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="160" spans="1:11" ht="31.5">
-      <c r="A160" s="22">
-        <v>41757</v>
+    <row r="160" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A160" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B160" s="24" t="s">
         <v>719</v>
@@ -10907,9 +10922,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="161" spans="1:86" ht="94.5">
-      <c r="A161" s="22">
-        <v>41757</v>
+    <row r="161" spans="1:86" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A161" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B161" s="24" t="s">
         <v>720</v>
@@ -10940,9 +10955,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="162" spans="1:86" ht="47.25">
-      <c r="A162" s="22">
-        <v>41757</v>
+    <row r="162" spans="1:86" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A162" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B162" s="24" t="s">
         <v>721</v>
@@ -10973,9 +10988,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="163" spans="1:86" ht="141.75">
-      <c r="A163" s="22">
-        <v>41757</v>
+    <row r="163" spans="1:86" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="A163" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B163" s="24" t="s">
         <v>722</v>
@@ -11002,9 +11017,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="164" spans="1:86" ht="94.5">
-      <c r="A164" s="22">
-        <v>41757</v>
+    <row r="164" spans="1:86" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A164" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B164" s="26" t="s">
         <v>723</v>
@@ -11033,9 +11048,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="165" spans="1:86" ht="94.5">
-      <c r="A165" s="22">
-        <v>41757</v>
+    <row r="165" spans="1:86" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A165" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B165" s="26" t="s">
         <v>724</v>
@@ -11064,9 +11079,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="166" spans="1:86" ht="94.5">
-      <c r="A166" s="22">
-        <v>41757</v>
+    <row r="166" spans="1:86" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A166" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B166" s="24" t="s">
         <v>725</v>
@@ -11093,9 +11108,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="167" spans="1:86" ht="94.5">
-      <c r="A167" s="22">
-        <v>41757</v>
+    <row r="167" spans="1:86" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A167" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B167" s="24" t="s">
         <v>726</v>
@@ -11122,9 +11137,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="168" spans="1:86" ht="94.5">
-      <c r="A168" s="22">
-        <v>41757</v>
+    <row r="168" spans="1:86" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A168" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B168" s="24" t="s">
         <v>727</v>
@@ -11151,9 +11166,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="169" spans="1:86" s="2" customFormat="1" ht="108" customHeight="1">
-      <c r="A169" s="22">
-        <v>41757</v>
+    <row r="169" spans="1:86" s="2" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B169" s="24" t="s">
         <v>728</v>
@@ -11255,9 +11270,9 @@
       <c r="CG169" s="3"/>
       <c r="CH169" s="3"/>
     </row>
-    <row r="170" spans="1:86" s="2" customFormat="1" ht="108" customHeight="1">
-      <c r="A170" s="22">
-        <v>41757</v>
+    <row r="170" spans="1:86" s="2" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A170" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B170" s="24" t="s">
         <v>729</v>
@@ -11359,9 +11374,9 @@
       <c r="CG170" s="3"/>
       <c r="CH170" s="3"/>
     </row>
-    <row r="171" spans="1:86" s="2" customFormat="1" ht="108" customHeight="1">
-      <c r="A171" s="22">
-        <v>41757</v>
+    <row r="171" spans="1:86" s="2" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A171" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B171" s="24" t="s">
         <v>730</v>
@@ -11463,9 +11478,9 @@
       <c r="CG171" s="3"/>
       <c r="CH171" s="3"/>
     </row>
-    <row r="172" spans="1:86" s="2" customFormat="1" ht="108" customHeight="1">
-      <c r="A172" s="22">
-        <v>41757</v>
+    <row r="172" spans="1:86" s="2" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A172" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B172" s="24" t="s">
         <v>731</v>
@@ -11567,9 +11582,9 @@
       <c r="CG172" s="3"/>
       <c r="CH172" s="3"/>
     </row>
-    <row r="173" spans="1:86" s="2" customFormat="1" ht="108" customHeight="1">
-      <c r="A173" s="22">
-        <v>41757</v>
+    <row r="173" spans="1:86" s="2" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A173" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B173" s="24" t="s">
         <v>732</v>
@@ -11671,9 +11686,9 @@
       <c r="CG173" s="3"/>
       <c r="CH173" s="3"/>
     </row>
-    <row r="174" spans="1:86" s="2" customFormat="1" ht="108" customHeight="1">
-      <c r="A174" s="22">
-        <v>41757</v>
+    <row r="174" spans="1:86" s="2" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A174" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B174" s="24" t="s">
         <v>733</v>
@@ -11775,9 +11790,9 @@
       <c r="CG174" s="3"/>
       <c r="CH174" s="3"/>
     </row>
-    <row r="175" spans="1:86" s="2" customFormat="1" ht="108" customHeight="1">
-      <c r="A175" s="22">
-        <v>41757</v>
+    <row r="175" spans="1:86" s="2" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A175" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B175" s="24" t="s">
         <v>734</v>
@@ -11879,9 +11894,9 @@
       <c r="CG175" s="3"/>
       <c r="CH175" s="3"/>
     </row>
-    <row r="176" spans="1:86" ht="94.5">
-      <c r="A176" s="22">
-        <v>41757</v>
+    <row r="176" spans="1:86" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A176" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B176" s="24" t="s">
         <v>735</v>
@@ -11908,9 +11923,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:86" s="13" customFormat="1" ht="105">
-      <c r="A177" s="22">
-        <v>41757</v>
+    <row r="177" spans="1:86" s="13" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A177" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B177" s="24" t="s">
         <v>736</v>
@@ -12012,9 +12027,9 @@
       <c r="CG177" s="14"/>
       <c r="CH177" s="14"/>
     </row>
-    <row r="178" spans="1:86" s="14" customFormat="1" ht="75">
-      <c r="A178" s="22">
-        <v>41757</v>
+    <row r="178" spans="1:86" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A178" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B178" s="24" t="s">
         <v>737</v>
@@ -12041,9 +12056,9 @@
         <v>484</v>
       </c>
     </row>
-    <row r="179" spans="1:86" s="13" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A179" s="22">
-        <v>41757</v>
+    <row r="179" spans="1:86" s="13" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A179" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B179" s="24" t="s">
         <v>738</v>
@@ -12149,9 +12164,9 @@
       <c r="CG179" s="14"/>
       <c r="CH179" s="14"/>
     </row>
-    <row r="180" spans="1:86" s="13" customFormat="1" ht="69" customHeight="1">
-      <c r="A180" s="22">
-        <v>41757</v>
+    <row r="180" spans="1:86" s="13" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A180" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B180" s="24" t="s">
         <v>739</v>
@@ -12257,9 +12272,9 @@
       <c r="CG180" s="14"/>
       <c r="CH180" s="14"/>
     </row>
-    <row r="181" spans="1:86" ht="63">
-      <c r="A181" s="22">
-        <v>41757</v>
+    <row r="181" spans="1:86" ht="63" x14ac:dyDescent="0.25">
+      <c r="A181" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B181" s="24" t="s">
         <v>740</v>
@@ -12286,9 +12301,9 @@
         <v>494</v>
       </c>
     </row>
-    <row r="182" spans="1:86" ht="63">
-      <c r="A182" s="22">
-        <v>41757</v>
+    <row r="182" spans="1:86" ht="63" x14ac:dyDescent="0.25">
+      <c r="A182" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B182" s="24" t="s">
         <v>741</v>
@@ -12315,9 +12330,9 @@
         <v>494</v>
       </c>
     </row>
-    <row r="183" spans="1:86" s="17" customFormat="1" ht="204.75">
-      <c r="A183" s="22">
-        <v>41757</v>
+    <row r="183" spans="1:86" s="17" customFormat="1" ht="204.75" x14ac:dyDescent="0.25">
+      <c r="A183" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B183" s="24" t="s">
         <v>742</v>
@@ -12423,9 +12438,9 @@
       <c r="CG183" s="18"/>
       <c r="CH183" s="18"/>
     </row>
-    <row r="184" spans="1:86" s="17" customFormat="1" ht="157.5">
-      <c r="A184" s="22">
-        <v>41757</v>
+    <row r="184" spans="1:86" s="17" customFormat="1" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A184" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B184" s="24" t="s">
         <v>743</v>
@@ -12531,9 +12546,9 @@
       <c r="CG184" s="18"/>
       <c r="CH184" s="18"/>
     </row>
-    <row r="185" spans="1:86" s="17" customFormat="1" ht="47.25">
-      <c r="A185" s="22">
-        <v>41757</v>
+    <row r="185" spans="1:86" s="17" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A185" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B185" s="24" t="s">
         <v>744</v>
@@ -12639,9 +12654,9 @@
       <c r="CG185" s="18"/>
       <c r="CH185" s="18"/>
     </row>
-    <row r="186" spans="1:86" s="17" customFormat="1" ht="94.5">
-      <c r="A186" s="22">
-        <v>41757</v>
+    <row r="186" spans="1:86" s="17" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A186" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B186" s="24" t="s">
         <v>745</v>
@@ -12747,9 +12762,9 @@
       <c r="CG186" s="18"/>
       <c r="CH186" s="18"/>
     </row>
-    <row r="187" spans="1:86" s="17" customFormat="1" ht="78.75">
-      <c r="A187" s="22">
-        <v>41757</v>
+    <row r="187" spans="1:86" s="17" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A187" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B187" s="24" t="s">
         <v>746</v>
@@ -12852,9 +12867,9 @@
       <c r="CG187" s="18"/>
       <c r="CH187" s="18"/>
     </row>
-    <row r="188" spans="1:86" s="17" customFormat="1" ht="47.25">
-      <c r="A188" s="22">
-        <v>41757</v>
+    <row r="188" spans="1:86" s="17" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A188" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B188" s="24" t="s">
         <v>747</v>
@@ -12960,9 +12975,9 @@
       <c r="CG188" s="18"/>
       <c r="CH188" s="18"/>
     </row>
-    <row r="189" spans="1:86" s="17" customFormat="1" ht="47.25">
-      <c r="A189" s="22">
-        <v>41757</v>
+    <row r="189" spans="1:86" s="17" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A189" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B189" s="24" t="s">
         <v>748</v>
@@ -13068,9 +13083,9 @@
       <c r="CG189" s="18"/>
       <c r="CH189" s="18"/>
     </row>
-    <row r="190" spans="1:86" s="17" customFormat="1" ht="110.25">
-      <c r="A190" s="22">
-        <v>41757</v>
+    <row r="190" spans="1:86" s="17" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A190" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B190" s="24" t="s">
         <v>749</v>
@@ -13176,9 +13191,9 @@
       <c r="CG190" s="18"/>
       <c r="CH190" s="18"/>
     </row>
-    <row r="191" spans="1:86" s="17" customFormat="1" ht="78.75">
-      <c r="A191" s="22">
-        <v>41757</v>
+    <row r="191" spans="1:86" s="17" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A191" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B191" s="24" t="s">
         <v>750</v>
@@ -13284,9 +13299,9 @@
       <c r="CG191" s="18"/>
       <c r="CH191" s="18"/>
     </row>
-    <row r="192" spans="1:86" s="17" customFormat="1" ht="157.5">
-      <c r="A192" s="22">
-        <v>41757</v>
+    <row r="192" spans="1:86" s="17" customFormat="1" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A192" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B192" s="24" t="s">
         <v>751</v>
@@ -13392,9 +13407,9 @@
       <c r="CG192" s="18"/>
       <c r="CH192" s="18"/>
     </row>
-    <row r="193" spans="1:86" s="17" customFormat="1" ht="110.25">
-      <c r="A193" s="22">
-        <v>41757</v>
+    <row r="193" spans="1:86" s="17" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A193" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B193" s="24" t="s">
         <v>752</v>
@@ -13494,9 +13509,9 @@
       <c r="CG193" s="18"/>
       <c r="CH193" s="18"/>
     </row>
-    <row r="194" spans="1:86" s="17" customFormat="1" ht="94.5">
-      <c r="A194" s="22">
-        <v>41757</v>
+    <row r="194" spans="1:86" s="17" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A194" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B194" s="24" t="s">
         <v>753</v>
@@ -13596,9 +13611,9 @@
       <c r="CG194" s="18"/>
       <c r="CH194" s="18"/>
     </row>
-    <row r="195" spans="1:86" s="17" customFormat="1" ht="126">
-      <c r="A195" s="22">
-        <v>41757</v>
+    <row r="195" spans="1:86" s="17" customFormat="1" ht="126" x14ac:dyDescent="0.25">
+      <c r="A195" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B195" s="24" t="s">
         <v>754</v>
@@ -13698,9 +13713,9 @@
       <c r="CG195" s="18"/>
       <c r="CH195" s="18"/>
     </row>
-    <row r="196" spans="1:86" s="17" customFormat="1" ht="110.25">
-      <c r="A196" s="22">
-        <v>41757</v>
+    <row r="196" spans="1:86" s="17" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A196" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B196" s="24" t="s">
         <v>755</v>
@@ -13800,9 +13815,9 @@
       <c r="CG196" s="18"/>
       <c r="CH196" s="18"/>
     </row>
-    <row r="197" spans="1:86" s="17" customFormat="1" ht="110.25">
-      <c r="A197" s="22">
-        <v>41757</v>
+    <row r="197" spans="1:86" s="17" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A197" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B197" s="24" t="s">
         <v>756</v>
@@ -13902,9 +13917,9 @@
       <c r="CG197" s="18"/>
       <c r="CH197" s="18"/>
     </row>
-    <row r="198" spans="1:86" s="17" customFormat="1" ht="110.25">
-      <c r="A198" s="22">
-        <v>41757</v>
+    <row r="198" spans="1:86" s="17" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A198" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B198" s="24" t="s">
         <v>757</v>
@@ -14004,9 +14019,9 @@
       <c r="CG198" s="18"/>
       <c r="CH198" s="18"/>
     </row>
-    <row r="199" spans="1:86" s="17" customFormat="1" ht="141.75">
-      <c r="A199" s="22">
-        <v>41757</v>
+    <row r="199" spans="1:86" s="17" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="A199" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B199" s="24" t="s">
         <v>758</v>
@@ -14106,9 +14121,9 @@
       <c r="CG199" s="18"/>
       <c r="CH199" s="18"/>
     </row>
-    <row r="200" spans="1:86" s="17" customFormat="1" ht="126">
-      <c r="A200" s="22">
-        <v>41757</v>
+    <row r="200" spans="1:86" s="17" customFormat="1" ht="126" x14ac:dyDescent="0.25">
+      <c r="A200" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B200" s="24" t="s">
         <v>759</v>
@@ -14208,9 +14223,9 @@
       <c r="CG200" s="18"/>
       <c r="CH200" s="18"/>
     </row>
-    <row r="201" spans="1:86" s="17" customFormat="1" ht="157.5">
-      <c r="A201" s="22">
-        <v>41757</v>
+    <row r="201" spans="1:86" s="17" customFormat="1" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A201" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B201" s="24" t="s">
         <v>760</v>
@@ -14316,9 +14331,9 @@
       <c r="CG201" s="18"/>
       <c r="CH201" s="18"/>
     </row>
-    <row r="202" spans="1:86" s="17" customFormat="1" ht="94.5">
-      <c r="A202" s="22">
-        <v>41757</v>
+    <row r="202" spans="1:86" s="17" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A202" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B202" s="24" t="s">
         <v>761</v>
@@ -14418,9 +14433,9 @@
       <c r="CG202" s="18"/>
       <c r="CH202" s="18"/>
     </row>
-    <row r="203" spans="1:86" s="17" customFormat="1" ht="63">
-      <c r="A203" s="22">
-        <v>41757</v>
+    <row r="203" spans="1:86" s="17" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A203" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B203" s="24" t="s">
         <v>762</v>
@@ -14526,9 +14541,9 @@
       <c r="CG203" s="18"/>
       <c r="CH203" s="18"/>
     </row>
-    <row r="204" spans="1:86" s="17" customFormat="1" ht="141.75">
-      <c r="A204" s="22">
-        <v>41757</v>
+    <row r="204" spans="1:86" s="17" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="A204" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B204" s="24" t="s">
         <v>763</v>
@@ -14634,9 +14649,9 @@
       <c r="CG204" s="18"/>
       <c r="CH204" s="18"/>
     </row>
-    <row r="205" spans="1:86" s="17" customFormat="1" ht="47.25">
-      <c r="A205" s="22">
-        <v>41757</v>
+    <row r="205" spans="1:86" s="17" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A205" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B205" s="24" t="s">
         <v>764</v>
@@ -14742,9 +14757,9 @@
       <c r="CG205" s="18"/>
       <c r="CH205" s="18"/>
     </row>
-    <row r="206" spans="1:86" s="17" customFormat="1" ht="47.25">
-      <c r="A206" s="22">
-        <v>41757</v>
+    <row r="206" spans="1:86" s="17" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A206" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B206" s="24" t="s">
         <v>765</v>
@@ -14850,9 +14865,9 @@
       <c r="CG206" s="18"/>
       <c r="CH206" s="18"/>
     </row>
-    <row r="207" spans="1:86" s="17" customFormat="1" ht="78.75">
-      <c r="A207" s="22">
-        <v>41757</v>
+    <row r="207" spans="1:86" s="17" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A207" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B207" s="26" t="s">
         <v>766</v>
@@ -14958,9 +14973,9 @@
       <c r="CG207" s="18"/>
       <c r="CH207" s="18"/>
     </row>
-    <row r="208" spans="1:86" s="17" customFormat="1" ht="141.75">
-      <c r="A208" s="22">
-        <v>41757</v>
+    <row r="208" spans="1:86" s="17" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="A208" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B208" s="24" t="s">
         <v>767</v>
@@ -15066,9 +15081,9 @@
       <c r="CG208" s="18"/>
       <c r="CH208" s="18"/>
     </row>
-    <row r="209" spans="1:86" s="17" customFormat="1" ht="167.25" customHeight="1">
-      <c r="A209" s="22">
-        <v>41757</v>
+    <row r="209" spans="1:86" s="17" customFormat="1" ht="167.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A209" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B209" s="24" t="s">
         <v>768</v>
@@ -15174,9 +15189,9 @@
       <c r="CG209" s="18"/>
       <c r="CH209" s="18"/>
     </row>
-    <row r="210" spans="1:86" s="17" customFormat="1" ht="78.75">
-      <c r="A210" s="22">
-        <v>41757</v>
+    <row r="210" spans="1:86" s="17" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A210" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B210" s="24" t="s">
         <v>769</v>
@@ -15282,9 +15297,9 @@
       <c r="CG210" s="18"/>
       <c r="CH210" s="18"/>
     </row>
-    <row r="211" spans="1:86" s="18" customFormat="1" ht="138" customHeight="1">
-      <c r="A211" s="22">
-        <v>41757</v>
+    <row r="211" spans="1:86" s="18" customFormat="1" ht="138" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A211" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B211" s="24" t="s">
         <v>770</v>
@@ -15315,9 +15330,9 @@
         <v>1338</v>
       </c>
     </row>
-    <row r="212" spans="1:86" s="18" customFormat="1" ht="181.5" customHeight="1">
-      <c r="A212" s="22">
-        <v>41757</v>
+    <row r="212" spans="1:86" s="18" customFormat="1" ht="181.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A212" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B212" s="24" t="s">
         <v>771</v>
@@ -15348,9 +15363,9 @@
         <v>1340</v>
       </c>
     </row>
-    <row r="213" spans="1:86" s="18" customFormat="1" ht="108" customHeight="1">
-      <c r="A213" s="22">
-        <v>41757</v>
+    <row r="213" spans="1:86" s="18" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A213" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B213" s="24" t="s">
         <v>772</v>
@@ -15381,9 +15396,9 @@
         <v>1342</v>
       </c>
     </row>
-    <row r="214" spans="1:86" s="18" customFormat="1" ht="96.75" customHeight="1">
-      <c r="A214" s="22">
-        <v>41757</v>
+    <row r="214" spans="1:86" s="18" customFormat="1" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A214" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B214" s="24" t="s">
         <v>773</v>
@@ -15414,9 +15429,9 @@
         <v>1242</v>
       </c>
     </row>
-    <row r="215" spans="1:86" s="18" customFormat="1" ht="117.75" customHeight="1">
-      <c r="A215" s="22">
-        <v>41757</v>
+    <row r="215" spans="1:86" s="18" customFormat="1" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A215" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B215" s="24" t="s">
         <v>774</v>
@@ -15447,9 +15462,9 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="216" spans="1:86" s="18" customFormat="1" ht="130.5" customHeight="1">
-      <c r="A216" s="22">
-        <v>41757</v>
+    <row r="216" spans="1:86" s="18" customFormat="1" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A216" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B216" s="24" t="s">
         <v>775</v>
@@ -15480,9 +15495,9 @@
         <v>1244</v>
       </c>
     </row>
-    <row r="217" spans="1:86" s="18" customFormat="1" ht="81.75" customHeight="1">
-      <c r="A217" s="22">
-        <v>41757</v>
+    <row r="217" spans="1:86" s="18" customFormat="1" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A217" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B217" s="24" t="s">
         <v>776</v>
@@ -15513,9 +15528,9 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="218" spans="1:86" s="17" customFormat="1" ht="94.5">
-      <c r="A218" s="22">
-        <v>41757</v>
+    <row r="218" spans="1:86" s="17" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A218" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B218" s="24" t="s">
         <v>777</v>
@@ -15621,9 +15636,9 @@
       <c r="CG218" s="18"/>
       <c r="CH218" s="18"/>
     </row>
-    <row r="219" spans="1:86" s="18" customFormat="1" ht="67.5" customHeight="1">
-      <c r="A219" s="22">
-        <v>41757</v>
+    <row r="219" spans="1:86" s="18" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A219" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B219" s="24" t="s">
         <v>778</v>
@@ -15654,9 +15669,9 @@
         <v>1318</v>
       </c>
     </row>
-    <row r="220" spans="1:86" s="18" customFormat="1" ht="209.25" customHeight="1">
-      <c r="A220" s="22">
-        <v>41757</v>
+    <row r="220" spans="1:86" s="18" customFormat="1" ht="209.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A220" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B220" s="24" t="s">
         <v>779</v>
@@ -15683,9 +15698,9 @@
         <v>560</v>
       </c>
     </row>
-    <row r="221" spans="1:86" s="19" customFormat="1" ht="101.25" customHeight="1">
-      <c r="A221" s="22">
-        <v>41757</v>
+    <row r="221" spans="1:86" s="19" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A221" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B221" s="24" t="s">
         <v>780</v>
@@ -15787,9 +15802,9 @@
       <c r="CG221" s="18"/>
       <c r="CH221" s="18"/>
     </row>
-    <row r="222" spans="1:86" s="20" customFormat="1" ht="94.5">
-      <c r="A222" s="22">
-        <v>41757</v>
+    <row r="222" spans="1:86" s="20" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A222" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B222" s="24" t="s">
         <v>781</v>
@@ -15891,9 +15906,9 @@
       <c r="CG222" s="21"/>
       <c r="CH222" s="21"/>
     </row>
-    <row r="223" spans="1:86" s="20" customFormat="1" ht="94.5">
-      <c r="A223" s="22">
-        <v>41757</v>
+    <row r="223" spans="1:86" s="20" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A223" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B223" s="24" t="s">
         <v>782</v>
@@ -15995,9 +16010,9 @@
       <c r="CG223" s="21"/>
       <c r="CH223" s="21"/>
     </row>
-    <row r="224" spans="1:86" s="20" customFormat="1" ht="94.5">
-      <c r="A224" s="22">
-        <v>41757</v>
+    <row r="224" spans="1:86" s="20" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A224" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B224" s="24" t="s">
         <v>783</v>
@@ -16099,9 +16114,9 @@
       <c r="CG224" s="21"/>
       <c r="CH224" s="21"/>
     </row>
-    <row r="225" spans="1:11" ht="225">
-      <c r="A225" s="23">
-        <v>41764</v>
+    <row r="225" spans="1:11" ht="225" x14ac:dyDescent="0.25">
+      <c r="A225" s="23" t="d">
+        <v>2014-05-05</v>
       </c>
       <c r="B225" s="24" t="s">
         <v>784</v>
@@ -16134,9 +16149,9 @@
         <v>822</v>
       </c>
     </row>
-    <row r="226" spans="1:11" ht="396" customHeight="1">
-      <c r="A226" s="23">
-        <v>41764</v>
+    <row r="226" spans="1:11" ht="396" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A226" s="23" t="d">
+        <v>2014-05-05</v>
       </c>
       <c r="B226" s="26" t="s">
         <v>785</v>
@@ -16169,9 +16184,9 @@
         <v>824</v>
       </c>
     </row>
-    <row r="227" spans="1:11" ht="270" customHeight="1">
-      <c r="A227" s="23">
-        <v>41764</v>
+    <row r="227" spans="1:11" ht="270" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A227" s="23" t="d">
+        <v>2014-05-05</v>
       </c>
       <c r="B227" s="26" t="s">
         <v>786</v>
@@ -16204,9 +16219,9 @@
         <v>826</v>
       </c>
     </row>
-    <row r="228" spans="1:11" ht="267" customHeight="1">
-      <c r="A228" s="23">
-        <v>41764</v>
+    <row r="228" spans="1:11" ht="267" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A228" s="23" t="d">
+        <v>2014-05-05</v>
       </c>
       <c r="B228" s="26" t="s">
         <v>787</v>
@@ -16239,9 +16254,9 @@
         <v>828</v>
       </c>
     </row>
-    <row r="229" spans="1:11" ht="384.75" customHeight="1">
-      <c r="A229" s="23">
-        <v>41764</v>
+    <row r="229" spans="1:11" ht="384.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A229" s="23" t="d">
+        <v>2014-05-05</v>
       </c>
       <c r="B229" s="26" t="s">
         <v>788</v>
@@ -16274,9 +16289,9 @@
         <v>833</v>
       </c>
     </row>
-    <row r="230" spans="1:11" ht="146.25" customHeight="1">
-      <c r="A230" s="23">
-        <v>41764</v>
+    <row r="230" spans="1:11" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A230" s="23" t="d">
+        <v>2014-05-05</v>
       </c>
       <c r="B230" s="26" t="s">
         <v>789</v>
@@ -16307,9 +16322,9 @@
         <v>885</v>
       </c>
     </row>
-    <row r="231" spans="1:11" ht="60">
-      <c r="A231" s="23">
-        <v>41764</v>
+    <row r="231" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A231" s="23" t="d">
+        <v>2014-05-05</v>
       </c>
       <c r="B231" s="26" t="s">
         <v>790</v>
@@ -16340,9 +16355,9 @@
         <v>886</v>
       </c>
     </row>
-    <row r="232" spans="1:11" ht="252" customHeight="1">
-      <c r="A232" s="23">
-        <v>41764</v>
+    <row r="232" spans="1:11" ht="252" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A232" s="23" t="d">
+        <v>2014-05-05</v>
       </c>
       <c r="B232" s="26" t="s">
         <v>791</v>
@@ -16375,9 +16390,9 @@
         <v>832</v>
       </c>
     </row>
-    <row r="233" spans="1:11" ht="90">
-      <c r="A233" s="23">
-        <v>41764</v>
+    <row r="233" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A233" s="23" t="d">
+        <v>2014-05-05</v>
       </c>
       <c r="B233" s="26" t="s">
         <v>792</v>
@@ -16408,9 +16423,9 @@
         <v>887</v>
       </c>
     </row>
-    <row r="234" spans="1:11" ht="75">
-      <c r="A234" s="23">
-        <v>41764</v>
+    <row r="234" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A234" s="23" t="d">
+        <v>2014-05-05</v>
       </c>
       <c r="B234" s="26" t="s">
         <v>793</v>
@@ -16441,9 +16456,9 @@
         <v>888</v>
       </c>
     </row>
-    <row r="235" spans="1:11" ht="60">
-      <c r="A235" s="23">
-        <v>41764</v>
+    <row r="235" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A235" s="23" t="d">
+        <v>2014-05-05</v>
       </c>
       <c r="B235" s="26" t="s">
         <v>794</v>
@@ -16474,9 +16489,9 @@
         <v>889</v>
       </c>
     </row>
-    <row r="236" spans="1:11" ht="240">
-      <c r="A236" s="23">
-        <v>41764</v>
+    <row r="236" spans="1:11" ht="255" x14ac:dyDescent="0.25">
+      <c r="A236" s="23" t="d">
+        <v>2014-05-05</v>
       </c>
       <c r="B236" s="26" t="s">
         <v>795</v>
@@ -16509,9 +16524,9 @@
         <v>852</v>
       </c>
     </row>
-    <row r="237" spans="1:11" ht="60">
-      <c r="A237" s="23">
-        <v>41764</v>
+    <row r="237" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A237" s="23" t="d">
+        <v>2014-05-05</v>
       </c>
       <c r="B237" s="26" t="s">
         <v>796</v>
@@ -16542,9 +16557,9 @@
         <v>890</v>
       </c>
     </row>
-    <row r="238" spans="1:11" ht="118.5" customHeight="1">
-      <c r="A238" s="23">
-        <v>41764</v>
+    <row r="238" spans="1:11" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A238" s="23" t="d">
+        <v>2014-05-05</v>
       </c>
       <c r="B238" s="26" t="s">
         <v>797</v>
@@ -16575,9 +16590,9 @@
         <v>891</v>
       </c>
     </row>
-    <row r="239" spans="1:11" ht="213.75" customHeight="1">
-      <c r="A239" s="23">
-        <v>41764</v>
+    <row r="239" spans="1:11" ht="213.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A239" s="23" t="d">
+        <v>2014-05-05</v>
       </c>
       <c r="B239" s="26" t="s">
         <v>798</v>
@@ -16610,9 +16625,9 @@
         <v>857</v>
       </c>
     </row>
-    <row r="240" spans="1:11" ht="60">
-      <c r="A240" s="23">
-        <v>41764</v>
+    <row r="240" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A240" s="23" t="d">
+        <v>2014-05-05</v>
       </c>
       <c r="B240" s="26" t="s">
         <v>799</v>
@@ -16643,9 +16658,9 @@
         <v>892</v>
       </c>
     </row>
-    <row r="241" spans="1:11" ht="330" customHeight="1">
-      <c r="A241" s="23">
-        <v>41764</v>
+    <row r="241" spans="1:11" ht="330" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A241" s="23" t="d">
+        <v>2014-05-05</v>
       </c>
       <c r="B241" s="26" t="s">
         <v>800</v>
@@ -16678,9 +16693,9 @@
         <v>858</v>
       </c>
     </row>
-    <row r="242" spans="1:11" ht="60">
-      <c r="A242" s="23">
-        <v>41764</v>
+    <row r="242" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A242" s="23" t="d">
+        <v>2014-05-05</v>
       </c>
       <c r="B242" s="26" t="s">
         <v>801</v>
@@ -16711,9 +16726,9 @@
         <v>893</v>
       </c>
     </row>
-    <row r="243" spans="1:11" ht="90">
-      <c r="A243" s="23">
-        <v>41764</v>
+    <row r="243" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A243" s="23" t="d">
+        <v>2014-05-05</v>
       </c>
       <c r="B243" s="26" t="s">
         <v>802</v>
@@ -16744,9 +16759,9 @@
         <v>894</v>
       </c>
     </row>
-    <row r="244" spans="1:11" ht="120">
-      <c r="A244" s="23">
-        <v>41764</v>
+    <row r="244" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="A244" s="23" t="d">
+        <v>2014-05-05</v>
       </c>
       <c r="B244" s="26" t="s">
         <v>803</v>
@@ -16777,9 +16792,9 @@
         <v>895</v>
       </c>
     </row>
-    <row r="245" spans="1:11" ht="331.5" customHeight="1">
-      <c r="A245" s="23">
-        <v>41764</v>
+    <row r="245" spans="1:11" ht="331.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A245" s="23" t="d">
+        <v>2014-05-05</v>
       </c>
       <c r="B245" s="26" t="s">
         <v>804</v>
@@ -16812,9 +16827,9 @@
         <v>884</v>
       </c>
     </row>
-    <row r="246" spans="1:11" s="1" customFormat="1" ht="258.75" customHeight="1">
-      <c r="A246" s="23">
-        <v>41764</v>
+    <row r="246" spans="1:11" s="1" customFormat="1" ht="258.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A246" s="23" t="d">
+        <v>2014-05-05</v>
       </c>
       <c r="B246" s="26" t="s">
         <v>805</v>
@@ -16847,9 +16862,9 @@
         <v>846</v>
       </c>
     </row>
-    <row r="247" spans="1:11" ht="391.5" customHeight="1">
-      <c r="A247" s="23">
-        <v>41768</v>
+    <row r="247" spans="1:11" ht="391.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A247" s="23" t="d">
+        <v>2014-05-09</v>
       </c>
       <c r="B247" s="26" t="s">
         <v>866</v>
@@ -16882,9 +16897,9 @@
         <v>872</v>
       </c>
     </row>
-    <row r="248" spans="1:11" ht="126">
-      <c r="A248" s="23">
-        <v>41772</v>
+    <row r="248" spans="1:11" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="A248" s="23" t="d">
+        <v>2014-05-13</v>
       </c>
       <c r="B248" s="26" t="s">
         <v>897</v>
@@ -16917,9 +16932,9 @@
         <v>906</v>
       </c>
     </row>
-    <row r="249" spans="1:11" ht="237.75" customHeight="1">
-      <c r="A249" s="23">
-        <v>41772</v>
+    <row r="249" spans="1:11" ht="237.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A249" s="23" t="d">
+        <v>2014-05-13</v>
       </c>
       <c r="B249" s="29" t="s">
         <v>907</v>
@@ -16952,9 +16967,9 @@
         <v>905</v>
       </c>
     </row>
-    <row r="250" spans="1:11" ht="190.5" customHeight="1">
-      <c r="A250" s="23">
-        <v>41772</v>
+    <row r="250" spans="1:11" ht="190.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A250" s="23" t="d">
+        <v>2014-05-13</v>
       </c>
       <c r="B250" s="35" t="s">
         <v>914</v>
@@ -16987,9 +17002,9 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="251" spans="1:11" ht="63">
-      <c r="A251" s="23">
-        <v>41772</v>
+    <row r="251" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A251" s="23" t="d">
+        <v>2014-05-13</v>
       </c>
       <c r="B251" s="29" t="s">
         <v>921</v>
@@ -17018,9 +17033,9 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="252" spans="1:11" ht="173.25">
-      <c r="A252" s="23">
-        <v>41772</v>
+    <row r="252" spans="1:11" ht="252" x14ac:dyDescent="0.25">
+      <c r="A252" s="23" t="d">
+        <v>2014-05-13</v>
       </c>
       <c r="B252" s="35" t="s">
         <v>925</v>
@@ -17053,9 +17068,9 @@
         <v>931</v>
       </c>
     </row>
-    <row r="253" spans="1:11" ht="325.5" customHeight="1">
-      <c r="A253" s="23">
-        <v>41772</v>
+    <row r="253" spans="1:11" ht="325.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A253" s="23" t="d">
+        <v>2014-05-13</v>
       </c>
       <c r="B253" s="35" t="s">
         <v>935</v>
@@ -17088,9 +17103,9 @@
         <v>939</v>
       </c>
     </row>
-    <row r="254" spans="1:11" ht="189">
-      <c r="A254" s="23">
-        <v>41772</v>
+    <row r="254" spans="1:11" ht="220.5" x14ac:dyDescent="0.25">
+      <c r="A254" s="23" t="d">
+        <v>2014-05-13</v>
       </c>
       <c r="B254" s="26" t="s">
         <v>940</v>
@@ -17123,9 +17138,9 @@
         <v>946</v>
       </c>
     </row>
-    <row r="255" spans="1:11" ht="308.25" customHeight="1">
-      <c r="A255" s="23">
-        <v>41772</v>
+    <row r="255" spans="1:11" ht="308.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A255" s="23" t="d">
+        <v>2014-05-13</v>
       </c>
       <c r="B255" s="26" t="s">
         <v>948</v>
@@ -17158,9 +17173,9 @@
         <v>953</v>
       </c>
     </row>
-    <row r="256" spans="1:11" ht="209.25" customHeight="1">
-      <c r="A256" s="23">
-        <v>41772</v>
+    <row r="256" spans="1:11" ht="209.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A256" s="23" t="d">
+        <v>2014-05-13</v>
       </c>
       <c r="B256" s="26" t="s">
         <v>954</v>
@@ -17193,9 +17208,9 @@
         <v>973</v>
       </c>
     </row>
-    <row r="257" spans="1:11" ht="190.5" customHeight="1">
-      <c r="A257" s="23">
-        <v>41772</v>
+    <row r="257" spans="1:11" ht="190.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A257" s="23" t="d">
+        <v>2014-05-13</v>
       </c>
       <c r="B257" s="26" t="s">
         <v>962</v>
@@ -17228,9 +17243,9 @@
         <v>963</v>
       </c>
     </row>
-    <row r="258" spans="1:11" ht="409.5" customHeight="1">
-      <c r="A258" s="23">
-        <v>41772</v>
+    <row r="258" spans="1:11" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A258" s="23" t="d">
+        <v>2014-05-13</v>
       </c>
       <c r="B258" s="26" t="s">
         <v>965</v>
@@ -17263,9 +17278,9 @@
         <v>976</v>
       </c>
     </row>
-    <row r="259" spans="1:11" ht="193.5" customHeight="1">
-      <c r="A259" s="23">
-        <v>41772</v>
+    <row r="259" spans="1:11" ht="193.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A259" s="23" t="d">
+        <v>2014-05-13</v>
       </c>
       <c r="B259" s="26" t="s">
         <v>967</v>
@@ -17298,9 +17313,9 @@
         <v>975</v>
       </c>
     </row>
-    <row r="260" spans="1:11" ht="250.5" customHeight="1">
-      <c r="A260" s="23">
-        <v>41772</v>
+    <row r="260" spans="1:11" ht="250.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A260" s="23" t="d">
+        <v>2014-05-13</v>
       </c>
       <c r="B260" s="26" t="s">
         <v>979</v>
@@ -17333,9 +17348,9 @@
         <v>984</v>
       </c>
     </row>
-    <row r="261" spans="1:11" ht="209.25" customHeight="1">
-      <c r="A261" s="23">
-        <v>41772</v>
+    <row r="261" spans="1:11" ht="209.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A261" s="23" t="d">
+        <v>2014-05-13</v>
       </c>
       <c r="B261" s="26" t="s">
         <v>986</v>
@@ -17368,9 +17383,9 @@
         <v>988</v>
       </c>
     </row>
-    <row r="262" spans="1:11" ht="261.75" customHeight="1">
-      <c r="A262" s="23">
-        <v>41772</v>
+    <row r="262" spans="1:11" ht="261.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A262" s="23" t="d">
+        <v>2014-05-13</v>
       </c>
       <c r="B262" s="35" t="s">
         <v>991</v>
@@ -17403,9 +17418,9 @@
         <v>997</v>
       </c>
     </row>
-    <row r="263" spans="1:11" ht="254.25" customHeight="1">
-      <c r="A263" s="23">
-        <v>41772</v>
+    <row r="263" spans="1:11" ht="254.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A263" s="23" t="d">
+        <v>2014-05-13</v>
       </c>
       <c r="B263" s="35" t="s">
         <v>1000</v>
@@ -17438,9 +17453,9 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="264" spans="1:11" ht="147.75" customHeight="1">
-      <c r="A264" s="23">
-        <v>41773</v>
+    <row r="264" spans="1:11" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A264" s="23" t="d">
+        <v>2014-05-14</v>
       </c>
       <c r="B264" s="38" t="s">
         <v>1006</v>
@@ -17471,9 +17486,9 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="265" spans="1:11" ht="318.75" customHeight="1">
-      <c r="A265" s="23">
-        <v>41775</v>
+    <row r="265" spans="1:11" ht="318.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A265" s="23" t="d">
+        <v>2014-05-16</v>
       </c>
       <c r="B265" s="35" t="s">
         <v>1014</v>
@@ -17502,9 +17517,9 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="266" spans="1:11" ht="240" customHeight="1">
-      <c r="A266" s="23">
-        <v>41775</v>
+    <row r="266" spans="1:11" ht="240" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A266" s="23" t="d">
+        <v>2014-05-16</v>
       </c>
       <c r="B266" s="35" t="s">
         <v>1025</v>
@@ -17537,9 +17552,9 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="267" spans="1:11" ht="147.75" customHeight="1">
-      <c r="A267" s="23">
-        <v>41775</v>
+    <row r="267" spans="1:11" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A267" s="23" t="d">
+        <v>2014-05-16</v>
       </c>
       <c r="B267" s="35" t="s">
         <v>1026</v>
@@ -17572,9 +17587,9 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="268" spans="1:11" ht="240.75" customHeight="1">
-      <c r="A268" s="23">
-        <v>41775</v>
+    <row r="268" spans="1:11" ht="240.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A268" s="23" t="d">
+        <v>2014-05-16</v>
       </c>
       <c r="B268" s="35" t="s">
         <v>1027</v>
@@ -17607,9 +17622,9 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="269" spans="1:11" ht="141.75">
-      <c r="A269" s="23">
-        <v>41775</v>
+    <row r="269" spans="1:11" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A269" s="23" t="d">
+        <v>2014-05-16</v>
       </c>
       <c r="B269" s="35" t="s">
         <v>1028</v>
@@ -17642,9 +17657,9 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="270" spans="1:11" ht="148.5" customHeight="1">
-      <c r="A270" s="23">
-        <v>41775</v>
+    <row r="270" spans="1:11" ht="148.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A270" s="23" t="d">
+        <v>2014-05-16</v>
       </c>
       <c r="B270" s="35" t="s">
         <v>1029</v>
@@ -17677,9 +17692,9 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="271" spans="1:11" ht="216.75" customHeight="1">
-      <c r="A271" s="23">
-        <v>41775</v>
+    <row r="271" spans="1:11" ht="216.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A271" s="23" t="d">
+        <v>2014-05-16</v>
       </c>
       <c r="B271" s="35" t="s">
         <v>1030</v>
@@ -17712,9 +17727,9 @@
         <v>1062</v>
       </c>
     </row>
-    <row r="272" spans="1:11" ht="94.5">
-      <c r="A272" s="23">
-        <v>41775</v>
+    <row r="272" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A272" s="23" t="d">
+        <v>2014-05-16</v>
       </c>
       <c r="B272" s="35" t="s">
         <v>1031</v>
@@ -17747,9 +17762,9 @@
         <v>1073</v>
       </c>
     </row>
-    <row r="273" spans="1:11" ht="257.25" customHeight="1">
-      <c r="A273" s="23">
-        <v>41775</v>
+    <row r="273" spans="1:11" ht="257.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A273" s="23" t="d">
+        <v>2014-05-16</v>
       </c>
       <c r="B273" s="35" t="s">
         <v>1032</v>
@@ -17782,9 +17797,9 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="274" spans="1:11" ht="102" customHeight="1">
-      <c r="A274" s="23">
-        <v>41775</v>
+    <row r="274" spans="1:11" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A274" s="23" t="d">
+        <v>2014-05-16</v>
       </c>
       <c r="B274" s="35" t="s">
         <v>1033</v>
@@ -17817,9 +17832,9 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="275" spans="1:11" ht="126">
-      <c r="A275" s="23">
-        <v>41775</v>
+    <row r="275" spans="1:11" ht="126" x14ac:dyDescent="0.25">
+      <c r="A275" s="23" t="d">
+        <v>2014-05-16</v>
       </c>
       <c r="B275" s="35" t="s">
         <v>1034</v>
@@ -17852,9 +17867,9 @@
         <v>1085</v>
       </c>
     </row>
-    <row r="276" spans="1:11" ht="126">
-      <c r="A276" s="23">
-        <v>41775</v>
+    <row r="276" spans="1:11" ht="126" x14ac:dyDescent="0.25">
+      <c r="A276" s="23" t="d">
+        <v>2014-05-16</v>
       </c>
       <c r="B276" s="35" t="s">
         <v>1035</v>
@@ -17887,9 +17902,9 @@
         <v>1088</v>
       </c>
     </row>
-    <row r="277" spans="1:11" ht="249.75" customHeight="1">
-      <c r="A277" s="23">
-        <v>41775</v>
+    <row r="277" spans="1:11" ht="249.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A277" s="23" t="d">
+        <v>2014-05-16</v>
       </c>
       <c r="B277" s="35" t="s">
         <v>1036</v>
@@ -17922,9 +17937,9 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="278" spans="1:11" ht="203.25" customHeight="1">
-      <c r="A278" s="23">
-        <v>41775</v>
+    <row r="278" spans="1:11" ht="203.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A278" s="23" t="d">
+        <v>2014-05-16</v>
       </c>
       <c r="B278" s="35" t="s">
         <v>1037</v>
@@ -17957,9 +17972,9 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="279" spans="1:11" ht="89.25" customHeight="1">
-      <c r="A279" s="23">
-        <v>41775</v>
+    <row r="279" spans="1:11" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A279" s="23" t="d">
+        <v>2014-05-16</v>
       </c>
       <c r="B279" s="35" t="s">
         <v>1038</v>
@@ -17992,9 +18007,9 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="280" spans="1:11" ht="126">
-      <c r="A280" s="23">
-        <v>41775</v>
+    <row r="280" spans="1:11" ht="126" x14ac:dyDescent="0.25">
+      <c r="A280" s="23" t="d">
+        <v>2014-05-16</v>
       </c>
       <c r="B280" s="35" t="s">
         <v>1101</v>
@@ -18027,9 +18042,9 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="281" spans="1:11" ht="157.5">
-      <c r="A281" s="23">
-        <v>41775</v>
+    <row r="281" spans="1:11" ht="189" x14ac:dyDescent="0.25">
+      <c r="A281" s="23" t="d">
+        <v>2014-05-16</v>
       </c>
       <c r="B281" s="35" t="s">
         <v>1102</v>
@@ -18062,9 +18077,9 @@
         <v>1117</v>
       </c>
     </row>
-    <row r="282" spans="1:11" ht="63">
-      <c r="A282" s="23">
-        <v>41775</v>
+    <row r="282" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A282" s="23" t="d">
+        <v>2014-05-16</v>
       </c>
       <c r="B282" s="35" t="s">
         <v>1103</v>
@@ -18084,9 +18099,9 @@
         <v>1116</v>
       </c>
     </row>
-    <row r="283" spans="1:11" ht="63">
-      <c r="A283" s="23">
-        <v>41775</v>
+    <row r="283" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A283" s="23" t="d">
+        <v>2014-05-16</v>
       </c>
       <c r="B283" s="35" t="s">
         <v>1104</v>
@@ -18106,9 +18121,9 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="284" spans="1:11" ht="220.5" customHeight="1">
-      <c r="A284" s="23">
-        <v>41775</v>
+    <row r="284" spans="1:11" ht="220.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A284" s="23" t="d">
+        <v>2014-05-16</v>
       </c>
       <c r="B284" s="35" t="s">
         <v>1105</v>
@@ -18137,9 +18152,9 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="285" spans="1:11" ht="168.75" customHeight="1">
-      <c r="A285" s="23">
-        <v>41775</v>
+    <row r="285" spans="1:11" ht="168.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A285" s="23" t="d">
+        <v>2014-05-16</v>
       </c>
       <c r="B285" s="35" t="s">
         <v>1106</v>
@@ -18172,9 +18187,9 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="286" spans="1:11" ht="141.75">
-      <c r="A286" s="23">
-        <v>41775</v>
+    <row r="286" spans="1:11" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="A286" s="23" t="d">
+        <v>2014-05-16</v>
       </c>
       <c r="B286" s="35" t="s">
         <v>1107</v>
@@ -18207,9 +18222,9 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="287" spans="1:11" ht="120" customHeight="1">
-      <c r="A287" s="23">
-        <v>41775</v>
+    <row r="287" spans="1:11" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A287" s="23" t="d">
+        <v>2014-05-16</v>
       </c>
       <c r="B287" s="35" t="s">
         <v>1108</v>
@@ -18242,9 +18257,9 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="288" spans="1:11" ht="126">
-      <c r="A288" s="23">
-        <v>41775</v>
+    <row r="288" spans="1:11" ht="126" x14ac:dyDescent="0.25">
+      <c r="A288" s="23" t="d">
+        <v>2014-05-16</v>
       </c>
       <c r="B288" s="35" t="s">
         <v>1109</v>
@@ -18277,9 +18292,9 @@
         <v>1152</v>
       </c>
     </row>
-    <row r="289" spans="1:11" ht="110.25">
-      <c r="A289" s="23">
-        <v>41775</v>
+    <row r="289" spans="1:11" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A289" s="23" t="d">
+        <v>2014-05-16</v>
       </c>
       <c r="B289" s="35" t="s">
         <v>1110</v>
@@ -18312,9 +18327,9 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="290" spans="1:11" ht="175.5" customHeight="1">
-      <c r="A290" s="23">
-        <v>41775</v>
+    <row r="290" spans="1:11" ht="175.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A290" s="23" t="d">
+        <v>2014-05-16</v>
       </c>
       <c r="B290" s="35" t="s">
         <v>1157</v>
@@ -18347,9 +18362,9 @@
         <v>1162</v>
       </c>
     </row>
-    <row r="291" spans="1:11" ht="126" customHeight="1">
-      <c r="A291" s="23">
-        <v>41775</v>
+    <row r="291" spans="1:11" ht="126" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A291" s="23" t="d">
+        <v>2014-05-16</v>
       </c>
       <c r="B291" s="35" t="s">
         <v>1158</v>
@@ -18382,9 +18397,9 @@
         <v>1165</v>
       </c>
     </row>
-    <row r="292" spans="1:11" ht="126">
-      <c r="A292" s="23">
-        <v>41775</v>
+    <row r="292" spans="1:11" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="A292" s="23" t="d">
+        <v>2014-05-16</v>
       </c>
       <c r="B292" s="35" t="s">
         <v>1159</v>
@@ -18417,9 +18432,9 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="293" spans="1:11" ht="236.25" customHeight="1">
-      <c r="A293" s="23">
-        <v>41775</v>
+    <row r="293" spans="1:11" ht="236.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A293" s="23" t="d">
+        <v>2014-05-16</v>
       </c>
       <c r="B293" s="35" t="s">
         <v>1160</v>
@@ -18452,9 +18467,9 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="294" spans="1:11" ht="31.5">
-      <c r="A294" s="45">
-        <v>41778</v>
+    <row r="294" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A294" s="45" t="d">
+        <v>2014-05-19</v>
       </c>
       <c r="B294" s="38" t="s">
         <v>1178</v>
@@ -18480,9 +18495,9 @@
         <v>1182</v>
       </c>
     </row>
-    <row r="295" spans="1:11" ht="31.5">
-      <c r="A295" s="45">
-        <v>41778</v>
+    <row r="295" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A295" s="45" t="d">
+        <v>2014-05-19</v>
       </c>
       <c r="B295" s="44" t="s">
         <v>1183</v>
@@ -18508,9 +18523,9 @@
         <v>1182</v>
       </c>
     </row>
-    <row r="296" spans="1:11" ht="31.5">
-      <c r="A296" s="45">
-        <v>41778</v>
+    <row r="296" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A296" s="45" t="d">
+        <v>2014-05-19</v>
       </c>
       <c r="B296" s="44" t="s">
         <v>1184</v>
@@ -18536,9 +18551,9 @@
         <v>1182</v>
       </c>
     </row>
-    <row r="297" spans="1:11" ht="34.5" customHeight="1">
-      <c r="A297" s="45">
-        <v>41778</v>
+    <row r="297" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A297" s="45" t="d">
+        <v>2014-05-19</v>
       </c>
       <c r="B297" s="38" t="s">
         <v>1185</v>
@@ -18564,9 +18579,9 @@
         <v>1182</v>
       </c>
     </row>
-    <row r="298" spans="1:11" ht="31.5">
-      <c r="A298" s="23">
-        <v>41781</v>
+    <row r="298" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A298" s="23" t="d">
+        <v>2014-05-22</v>
       </c>
       <c r="B298" s="35" t="s">
         <v>1345</v>
@@ -18597,9 +18612,9 @@
         <v>1344</v>
       </c>
     </row>
-    <row r="299" spans="1:11" ht="63">
-      <c r="A299" s="23">
-        <v>41781</v>
+    <row r="299" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A299" s="23" t="d">
+        <v>2014-05-22</v>
       </c>
       <c r="B299" s="35" t="s">
         <v>1348</v>
@@ -18630,9 +18645,9 @@
         <v>1347</v>
       </c>
     </row>
-    <row r="300" spans="1:11" ht="47.25">
-      <c r="A300" s="23">
-        <v>41781</v>
+    <row r="300" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A300" s="23" t="d">
+        <v>2014-05-22</v>
       </c>
       <c r="B300" s="35" t="s">
         <v>1349</v>
@@ -18663,9 +18678,9 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="301" spans="1:11" ht="63">
-      <c r="A301" s="23">
-        <v>41781</v>
+    <row r="301" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A301" s="23" t="d">
+        <v>2014-05-22</v>
       </c>
       <c r="B301" s="35" t="s">
         <v>1353</v>
@@ -18692,9 +18707,9 @@
         <v>1355</v>
       </c>
     </row>
-    <row r="302" spans="1:11" ht="63">
-      <c r="A302" s="23">
-        <v>41781</v>
+    <row r="302" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A302" s="23" t="d">
+        <v>2014-05-22</v>
       </c>
       <c r="B302" s="35" t="s">
         <v>1362</v>
@@ -18723,9 +18738,9 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="303" spans="1:11" ht="63">
-      <c r="A303" s="23">
-        <v>41781</v>
+    <row r="303" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A303" s="23" t="d">
+        <v>2014-05-22</v>
       </c>
       <c r="B303" s="35" t="s">
         <v>1363</v>
@@ -18754,9 +18769,9 @@
         <v>1365</v>
       </c>
     </row>
-    <row r="304" spans="1:11" ht="63">
-      <c r="A304" s="23">
-        <v>41781</v>
+    <row r="304" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A304" s="23" t="d">
+        <v>2014-05-22</v>
       </c>
       <c r="B304" s="35" t="s">
         <v>1366</v>
@@ -18785,9 +18800,9 @@
         <v>1368</v>
       </c>
     </row>
-    <row r="305" spans="1:11" ht="63">
-      <c r="A305" s="23">
-        <v>41781</v>
+    <row r="305" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A305" s="23" t="d">
+        <v>2014-05-22</v>
       </c>
       <c r="B305" s="35" t="s">
         <v>1369</v>
@@ -18816,9 +18831,9 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="306" spans="1:11" ht="63">
-      <c r="A306" s="23">
-        <v>41781</v>
+    <row r="306" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A306" s="23" t="d">
+        <v>2014-05-22</v>
       </c>
       <c r="B306" s="35" t="s">
         <v>1374</v>
@@ -18847,9 +18862,9 @@
         <v>1373</v>
       </c>
     </row>
-    <row r="307" spans="1:11" ht="63">
-      <c r="A307" s="23">
-        <v>41781</v>
+    <row r="307" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A307" s="23" t="d">
+        <v>2014-05-22</v>
       </c>
       <c r="B307" s="35" t="s">
         <v>1375</v>
@@ -18878,9 +18893,9 @@
         <v>1377</v>
       </c>
     </row>
-    <row r="308" spans="1:11" ht="63">
-      <c r="A308" s="23">
-        <v>41781</v>
+    <row r="308" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A308" s="23" t="d">
+        <v>2014-05-22</v>
       </c>
       <c r="B308" s="35" t="s">
         <v>1378</v>
@@ -18909,9 +18924,9 @@
         <v>1380</v>
       </c>
     </row>
-    <row r="309" spans="1:11" ht="63">
-      <c r="A309" s="23">
-        <v>41781</v>
+    <row r="309" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A309" s="23" t="d">
+        <v>2014-05-22</v>
       </c>
       <c r="B309" s="35" t="s">
         <v>1381</v>
@@ -18940,9 +18955,9 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="310" spans="1:11" ht="78.75">
-      <c r="A310" s="23">
-        <v>41781</v>
+    <row r="310" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A310" s="23" t="d">
+        <v>2014-05-22</v>
       </c>
       <c r="B310" s="35" t="s">
         <v>1384</v>
@@ -18971,9 +18986,9 @@
         <v>1386</v>
       </c>
     </row>
-    <row r="311" spans="1:11" ht="78.75">
-      <c r="A311" s="23">
-        <v>41781</v>
+    <row r="311" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A311" s="23" t="d">
+        <v>2014-05-22</v>
       </c>
       <c r="B311" s="35" t="s">
         <v>1387</v>
@@ -19004,9 +19019,9 @@
         <v>1393</v>
       </c>
     </row>
-    <row r="312" spans="1:11" ht="63">
-      <c r="A312" s="23">
-        <v>41781</v>
+    <row r="312" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A312" s="23" t="d">
+        <v>2014-05-22</v>
       </c>
       <c r="B312" s="35" t="s">
         <v>1394</v>
@@ -19037,9 +19052,9 @@
         <v>1397</v>
       </c>
     </row>
-    <row r="313" spans="1:11" ht="63">
-      <c r="A313" s="23">
-        <v>41781</v>
+    <row r="313" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A313" s="23" t="d">
+        <v>2014-05-22</v>
       </c>
       <c r="B313" s="35" t="s">
         <v>1395</v>
@@ -19070,9 +19085,9 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="314" spans="1:11" ht="47.25">
-      <c r="A314" s="23">
-        <v>41781</v>
+    <row r="314" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A314" s="23" t="d">
+        <v>2014-05-22</v>
       </c>
       <c r="B314" s="35" t="s">
         <v>1396</v>
@@ -19103,9 +19118,9 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="315" spans="1:11" ht="47.25">
-      <c r="A315" s="23">
-        <v>41781</v>
+    <row r="315" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A315" s="23" t="d">
+        <v>2014-05-22</v>
       </c>
       <c r="B315" s="35" t="s">
         <v>1403</v>
@@ -19136,9 +19151,9 @@
         <v>1407</v>
       </c>
     </row>
-    <row r="316" spans="1:11" ht="78.75">
-      <c r="A316" s="23">
-        <v>41781</v>
+    <row r="316" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A316" s="23" t="d">
+        <v>2014-05-22</v>
       </c>
       <c r="B316" s="35" t="s">
         <v>1409</v>
@@ -19169,9 +19184,9 @@
         <v>1410</v>
       </c>
     </row>
-    <row r="317" spans="1:11" ht="47.25">
-      <c r="A317" s="23">
-        <v>41781</v>
+    <row r="317" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A317" s="23" t="d">
+        <v>2014-05-22</v>
       </c>
       <c r="B317" s="35" t="s">
         <v>1411</v>
@@ -19202,18 +19217,12 @@
         <v>1402</v>
       </c>
     </row>
-    <row r="318" spans="1:11">
+    <row r="318" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A318" s="23"/>
       <c r="B318" s="35"/>
     </row>
   </sheetData>
   <autoFilter ref="D1:K317">
-    <filterColumn colId="0"/>
-    <filterColumn colId="1"/>
-    <filterColumn colId="2"/>
-    <filterColumn colId="4"/>
-    <filterColumn colId="5"/>
-    <filterColumn colId="6"/>
     <sortState ref="D2:K283">
       <sortCondition ref="D1:D283"/>
     </sortState>
@@ -19231,14 +19240,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" style="11" customWidth="1"/>
     <col min="2" max="2" width="23" style="11" customWidth="1"/>
@@ -19251,7 +19260,7 @@
     <col min="9" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="25.5" customHeight="1">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>496</v>
       </c>
@@ -19277,9 +19286,9 @@
         <v>436</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="3" customFormat="1" ht="94.5">
-      <c r="A2" s="22">
-        <v>41757</v>
+    <row r="2" spans="1:8" s="3" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B2" s="22" t="s">
         <v>808</v>
@@ -19303,9 +19312,9 @@
         <v>447</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="3" customFormat="1" ht="78.75">
-      <c r="A3" s="22">
-        <v>41757</v>
+    <row r="3" spans="1:8" s="3" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B3" s="22" t="s">
         <v>809</v>
@@ -19329,9 +19338,9 @@
         <v>449</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="3" customFormat="1" ht="141.75">
-      <c r="A4" s="22">
-        <v>41757</v>
+    <row r="4" spans="1:8" s="3" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B4" s="22" t="s">
         <v>810</v>
@@ -19355,9 +19364,9 @@
         <v>451</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="1" customFormat="1" ht="126">
-      <c r="A5" s="22">
-        <v>41757</v>
+    <row r="5" spans="1:8" s="1" customFormat="1" ht="126" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B5" s="22" t="s">
         <v>811</v>
@@ -19381,9 +19390,9 @@
         <v>453</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="1" customFormat="1" ht="283.5">
-      <c r="A6" s="22">
-        <v>41757</v>
+    <row r="6" spans="1:8" s="1" customFormat="1" ht="283.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B6" s="22" t="s">
         <v>812</v>
@@ -19407,9 +19416,9 @@
         <v>455</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="1" customFormat="1" ht="126">
-      <c r="A7" s="22">
-        <v>41757</v>
+    <row r="7" spans="1:8" s="1" customFormat="1" ht="126" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B7" s="22" t="s">
         <v>813</v>
@@ -19433,9 +19442,9 @@
         <v>457</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="1" customFormat="1" ht="330.75">
-      <c r="A8" s="22">
-        <v>41757</v>
+    <row r="8" spans="1:8" s="1" customFormat="1" ht="330.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B8" s="22" t="s">
         <v>815</v>
@@ -19459,9 +19468,9 @@
         <v>459</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="1" customFormat="1" ht="236.25">
-      <c r="A9" s="22">
-        <v>41757</v>
+    <row r="9" spans="1:8" s="1" customFormat="1" ht="236.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B9" s="22" t="s">
         <v>814</v>
@@ -19485,9 +19494,9 @@
         <v>461</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="1" customFormat="1" ht="94.5">
-      <c r="A10" s="22">
-        <v>41757</v>
+    <row r="10" spans="1:8" s="1" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B10" s="22" t="s">
         <v>816</v>
@@ -19511,9 +19520,9 @@
         <v>463</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="1" customFormat="1" ht="110.25">
-      <c r="A11" s="22">
-        <v>41757</v>
+    <row r="11" spans="1:8" s="1" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B11" s="22" t="s">
         <v>817</v>
@@ -19537,9 +19546,9 @@
         <v>465</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="1" customFormat="1" ht="63">
-      <c r="A12" s="22">
-        <v>41757</v>
+    <row r="12" spans="1:8" s="1" customFormat="1" ht="63" x14ac:dyDescent="0.25">
+      <c r="A12" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B12" s="22" t="s">
         <v>818</v>
@@ -19563,9 +19572,9 @@
         <v>467</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="1" customFormat="1" ht="110.25">
-      <c r="A13" s="22">
-        <v>41757</v>
+    <row r="13" spans="1:8" s="1" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B13" s="22" t="s">
         <v>819</v>
@@ -19589,9 +19598,9 @@
         <v>469</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="1" customFormat="1" ht="94.5">
-      <c r="A14" s="22">
-        <v>41757</v>
+    <row r="14" spans="1:8" s="1" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="d">
+        <v>2014-04-28</v>
       </c>
       <c r="B14" s="22" t="s">
         <v>820</v>
@@ -19615,7 +19624,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="22"/>
       <c r="B15" s="22"/>
     </row>
@@ -19633,19 +19642,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="11" max="11" width="45.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="11:11" ht="195" customHeight="1">
+    <row r="1" spans="11:11" ht="195" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K1" s="3" t="s">
         <v>932</v>
       </c>
@@ -19656,14 +19665,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="2" width="23.42578125" customWidth="1"/>

</xml_diff>